<commit_message>
Verified Benjy Renton data and added citation to README
</commit_message>
<xml_diff>
--- a/clemsonDashboard.xlsx
+++ b/clemsonDashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidferrara/Documents/Clemson/The Tiger/COVID-19/Data/ttn-clemson-covid-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1156C155-0CBC-1E41-9666-84174CA5CCD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AC0A9D-7180-564A-BCCF-9BF51BA288A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16260" xr2:uid="{663FE1B6-0B7E-E04A-924C-6AB15F4F5852}"/>
   </bookViews>
@@ -209,7 +209,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000%"/>
-    <numFmt numFmtId="170" formatCode="m/d;@"/>
+    <numFmt numFmtId="165" formatCode="m/d;@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -318,25 +318,25 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -717,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2018E299-360B-F244-BDDD-9B449D0B7C0F}">
   <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1156,7 +1156,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="7">
-        <f t="shared" ref="G29:G36" si="0">B29+G28</f>
+        <f>B29+G28</f>
         <v>2326</v>
       </c>
     </row>
@@ -1168,7 +1168,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="7">
-        <f t="shared" si="0"/>
+        <f>B30+G29</f>
         <v>2329</v>
       </c>
     </row>
@@ -1180,7 +1180,7 @@
         <v>93</v>
       </c>
       <c r="G31" s="7">
-        <f t="shared" si="0"/>
+        <f>B31+G30</f>
         <v>2422</v>
       </c>
     </row>
@@ -1192,7 +1192,7 @@
         <v>34</v>
       </c>
       <c r="G32" s="7">
-        <f t="shared" si="0"/>
+        <f>B32+G31</f>
         <v>2456</v>
       </c>
     </row>
@@ -1204,7 +1204,7 @@
         <v>73</v>
       </c>
       <c r="G33" s="7">
-        <f t="shared" si="0"/>
+        <f>B33+G32</f>
         <v>2529</v>
       </c>
     </row>
@@ -1216,7 +1216,7 @@
         <v>116</v>
       </c>
       <c r="G34" s="7">
-        <f t="shared" si="0"/>
+        <f>B34+G33</f>
         <v>2645</v>
       </c>
     </row>
@@ -1228,7 +1228,7 @@
         <v>92</v>
       </c>
       <c r="G35" s="7">
-        <f t="shared" si="0"/>
+        <f>B35+G34</f>
         <v>2737</v>
       </c>
     </row>
@@ -1240,7 +1240,7 @@
         <v>72</v>
       </c>
       <c r="G36" s="7">
-        <f t="shared" si="0"/>
+        <f>B36+G35</f>
         <v>2809</v>
       </c>
     </row>
@@ -1255,12 +1255,12 @@
         <v>401</v>
       </c>
       <c r="E37" s="4">
-        <f t="shared" ref="E37:E64" si="1">B37/D37</f>
+        <f>B37/D37</f>
         <v>2.2443890274314215E-2</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="7">
-        <f t="shared" ref="G37:G64" si="2">B37+G36</f>
+        <f>B37+G36</f>
         <v>2818</v>
       </c>
       <c r="H37">
@@ -1292,7 +1292,7 @@
         <v>112</v>
       </c>
       <c r="Q37" t="str">
-        <f t="shared" ref="Q37:Q64" si="3">IF(I37+K37=B37,"EQUAL","DIFFER")</f>
+        <f>IF(I37+K37=B37,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R37" t="str">
@@ -1319,16 +1319,16 @@
         <v>2170</v>
       </c>
       <c r="E38" s="4">
-        <f t="shared" si="1"/>
+        <f>B38/D38</f>
         <v>8.4792626728110596E-2</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="7">
-        <f t="shared" si="2"/>
+        <f>B38+G37</f>
         <v>3002</v>
       </c>
       <c r="H38">
-        <f t="shared" ref="H38:H64" si="4">H37+D38</f>
+        <f t="shared" ref="H38:H64" si="0">H37+D38</f>
         <v>2571</v>
       </c>
       <c r="I38">
@@ -1356,19 +1356,19 @@
         <v>45</v>
       </c>
       <c r="Q38" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I38+K38=B38,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R38" t="str">
-        <f t="shared" ref="R38:R64" si="5">IF(J38+L38=D38,"EQUAL","DIFFER")</f>
+        <f t="shared" ref="R38:R64" si="1">IF(J38+L38=D38,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="S38" t="str">
-        <f t="shared" ref="S38:S63" si="6">IF(M38+O38=B38,"EQUAL","DIFFER")</f>
+        <f>IF(M38+O38=B38,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T38" t="str">
-        <f t="shared" ref="T38:T64" si="7">IF(N38+P38=D38,"EQUAL","DIFFER")</f>
+        <f t="shared" ref="T38:T64" si="2">IF(N38+P38=D38,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
     </row>
@@ -1383,16 +1383,16 @@
         <v>1272</v>
       </c>
       <c r="E39" s="4">
-        <f t="shared" si="1"/>
+        <f>B39/D39</f>
         <v>5.4245283018867926E-2</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="7">
-        <f t="shared" si="2"/>
+        <f>B39+G38</f>
         <v>3071</v>
       </c>
       <c r="H39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>3843</v>
       </c>
       <c r="I39">
@@ -1420,19 +1420,19 @@
         <v>42</v>
       </c>
       <c r="Q39" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I39+K39=B39,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R39" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S39" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M39+O39=B39,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T39" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -1447,16 +1447,16 @@
         <v>2062</v>
       </c>
       <c r="E40" s="4">
-        <f t="shared" si="1"/>
+        <f>B40/D40</f>
         <v>7.953443258971872E-2</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="7">
-        <f t="shared" si="2"/>
+        <f>B40+G39</f>
         <v>3235</v>
       </c>
       <c r="H40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>5905</v>
       </c>
       <c r="I40">
@@ -1484,19 +1484,19 @@
         <v>169</v>
       </c>
       <c r="Q40" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I40+K40=B40,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S40" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M40+O40=B40,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -1511,16 +1511,16 @@
         <v>1210</v>
       </c>
       <c r="E41" s="4">
-        <f t="shared" si="1"/>
+        <f>B41/D41</f>
         <v>7.1074380165289261E-2</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="7">
-        <f t="shared" si="2"/>
+        <f>B41+G40</f>
         <v>3321</v>
       </c>
       <c r="H41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>7115</v>
       </c>
       <c r="I41">
@@ -1548,19 +1548,19 @@
         <v>37</v>
       </c>
       <c r="Q41" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I41+K41=B41,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R41" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S41" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M41+O41=B41,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -1575,16 +1575,16 @@
         <v>1618</v>
       </c>
       <c r="E42" s="4">
-        <f t="shared" si="1"/>
+        <f>B42/D42</f>
         <v>4.3263288009888753E-2</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="7">
-        <f t="shared" si="2"/>
+        <f>B42+G41</f>
         <v>3391</v>
       </c>
       <c r="H42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>8733</v>
       </c>
       <c r="I42">
@@ -1612,19 +1612,19 @@
         <v>279</v>
       </c>
       <c r="Q42" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I42+K42=B42,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R42" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S42" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M42+O42=B42,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T42" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -1639,16 +1639,16 @@
         <v>20</v>
       </c>
       <c r="E43" s="4">
-        <f t="shared" si="1"/>
+        <f>B43/D43</f>
         <v>0.3</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="7">
-        <f t="shared" si="2"/>
+        <f>B43+G42</f>
         <v>3397</v>
       </c>
       <c r="H43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>8753</v>
       </c>
       <c r="I43">
@@ -1676,19 +1676,19 @@
         <v>1</v>
       </c>
       <c r="Q43" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I43+K43=B43,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R43" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S43" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M43+O43=B43,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T43" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -1703,16 +1703,16 @@
         <v>309</v>
       </c>
       <c r="E44" s="4">
-        <f t="shared" si="1"/>
+        <f>B44/D44</f>
         <v>1.2944983818770227E-2</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="7">
-        <f t="shared" si="2"/>
+        <f>B44+G43</f>
         <v>3401</v>
       </c>
       <c r="H44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>9062</v>
       </c>
       <c r="I44">
@@ -1740,19 +1740,19 @@
         <v>99</v>
       </c>
       <c r="Q44" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I44+K44=B44,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R44" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S44" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M44+O44=B44,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -1767,16 +1767,16 @@
         <v>1716</v>
       </c>
       <c r="E45" s="4">
-        <f t="shared" si="1"/>
+        <f>B45/D45</f>
         <v>5.7109557109557112E-2</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="7">
-        <f t="shared" si="2"/>
+        <f>B45+G44</f>
         <v>3499</v>
       </c>
       <c r="H45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>10778</v>
       </c>
       <c r="I45">
@@ -1804,19 +1804,19 @@
         <v>174</v>
       </c>
       <c r="Q45" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I45+K45=B45,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R45" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S45" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M45+O45=B45,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T45" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -1831,16 +1831,16 @@
         <v>1251</v>
       </c>
       <c r="E46" s="4">
-        <f t="shared" si="1"/>
+        <f>B46/D46</f>
         <v>6.7146282973621102E-2</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="7">
-        <f t="shared" si="2"/>
+        <f>B46+G45</f>
         <v>3583</v>
       </c>
       <c r="H46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>12029</v>
       </c>
       <c r="I46">
@@ -1868,19 +1868,19 @@
         <v>114</v>
       </c>
       <c r="Q46" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I46+K46=B46,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R46" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S46" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M46+O46=B46,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T46" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -1895,16 +1895,16 @@
         <v>2690</v>
       </c>
       <c r="E47" s="4">
-        <f t="shared" si="1"/>
+        <f>B47/D47</f>
         <v>3.1226765799256505E-2</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="7">
-        <f t="shared" si="2"/>
+        <f>B47+G46</f>
         <v>3667</v>
       </c>
       <c r="H47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>14719</v>
       </c>
       <c r="I47">
@@ -1932,19 +1932,19 @@
         <v>454</v>
       </c>
       <c r="Q47" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I47+K47=B47,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S47" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M47+O47=B47,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T47" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -1959,16 +1959,16 @@
         <v>1374</v>
       </c>
       <c r="E48" s="4">
-        <f t="shared" si="1"/>
+        <f>B48/D48</f>
         <v>3.7117903930131008E-2</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="7">
-        <f t="shared" si="2"/>
+        <f>B48+G47</f>
         <v>3718</v>
       </c>
       <c r="H48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>16093</v>
       </c>
       <c r="I48">
@@ -1996,19 +1996,19 @@
         <v>111</v>
       </c>
       <c r="Q48" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I48+K48=B48,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S48" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M48+O48=B48,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T48" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2023,16 +2023,16 @@
         <v>1601</v>
       </c>
       <c r="E49" s="4">
-        <f t="shared" si="1"/>
+        <f>B49/D49</f>
         <v>4.996876951905059E-2</v>
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="7">
-        <f t="shared" si="2"/>
+        <f>B49+G48</f>
         <v>3798</v>
       </c>
       <c r="H49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>17694</v>
       </c>
       <c r="I49">
@@ -2060,19 +2060,19 @@
         <v>149</v>
       </c>
       <c r="Q49" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I49+K49=B49,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R49" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S49" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M49+O49=B49,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T49" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2087,16 +2087,16 @@
         <v>282</v>
       </c>
       <c r="E50" s="4">
-        <f t="shared" si="1"/>
+        <f>B50/D50</f>
         <v>2.1276595744680851E-2</v>
       </c>
       <c r="F50" s="4"/>
       <c r="G50" s="7">
-        <f t="shared" si="2"/>
+        <f>B50+G49</f>
         <v>3804</v>
       </c>
       <c r="H50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>17976</v>
       </c>
       <c r="I50">
@@ -2124,19 +2124,19 @@
         <v>66</v>
       </c>
       <c r="Q50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I50+K50=B50,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R50" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S50" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M50+O50=B50,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T50" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2151,16 +2151,16 @@
         <v>270</v>
       </c>
       <c r="E51" s="4">
-        <f t="shared" si="1"/>
+        <f>B51/D51</f>
         <v>1.8518518518518517E-2</v>
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="7">
-        <f t="shared" si="2"/>
+        <f>B51+G50</f>
         <v>3809</v>
       </c>
       <c r="H51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>18246</v>
       </c>
       <c r="I51">
@@ -2188,19 +2188,19 @@
         <v>90</v>
       </c>
       <c r="Q51" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I51+K51=B51,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R51" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S51" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M51+O51=B51,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T51" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2215,16 +2215,16 @@
         <v>1606</v>
       </c>
       <c r="E52" s="4">
-        <f t="shared" si="1"/>
+        <f>B52/D52</f>
         <v>5.7285180572851806E-2</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="7">
-        <f t="shared" si="2"/>
+        <f>B52+G51</f>
         <v>3901</v>
       </c>
       <c r="H52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>19852</v>
       </c>
       <c r="I52">
@@ -2252,19 +2252,19 @@
         <v>247</v>
       </c>
       <c r="Q52" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I52+K52=B52,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R52" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S52" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M52+O52=B52,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T52" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2279,16 +2279,16 @@
         <v>1714</v>
       </c>
       <c r="E53" s="4">
-        <f t="shared" si="1"/>
+        <f>B53/D53</f>
         <v>2.8588098016336057E-2</v>
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="7">
-        <f t="shared" si="2"/>
+        <f>B53+G52</f>
         <v>3950</v>
       </c>
       <c r="H53">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>21566</v>
       </c>
       <c r="I53">
@@ -2316,19 +2316,19 @@
         <v>122</v>
       </c>
       <c r="Q53" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I53+K53=B53,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R53" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S53" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M53+O53=B53,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T53" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2343,16 +2343,16 @@
         <v>2925</v>
       </c>
       <c r="E54" s="4">
-        <f t="shared" si="1"/>
+        <f>B54/D54</f>
         <v>1.5726495726495728E-2</v>
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="7">
-        <f t="shared" si="2"/>
+        <f>B54+G53</f>
         <v>3996</v>
       </c>
       <c r="H54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>24491</v>
       </c>
       <c r="I54">
@@ -2380,19 +2380,19 @@
         <v>348</v>
       </c>
       <c r="Q54" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I54+K54=B54,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R54" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S54" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M54+O54=B54,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2407,16 +2407,16 @@
         <v>1690</v>
       </c>
       <c r="E55" s="4">
-        <f t="shared" si="1"/>
+        <f>B55/D55</f>
         <v>1.242603550295858E-2</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="7">
-        <f t="shared" si="2"/>
+        <f>B55+G54</f>
         <v>4017</v>
       </c>
       <c r="H55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>26181</v>
       </c>
       <c r="I55">
@@ -2444,19 +2444,19 @@
         <v>75</v>
       </c>
       <c r="Q55" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I55+K55=B55,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R55" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S55" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M55+O55=B55,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T55" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2471,16 +2471,16 @@
         <v>813</v>
       </c>
       <c r="E56" s="4">
-        <f t="shared" si="1"/>
+        <f>B56/D56</f>
         <v>4.0590405904059039E-2</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="7">
-        <f t="shared" si="2"/>
+        <f>B56+G55</f>
         <v>4050</v>
       </c>
       <c r="H56">
-        <f t="shared" si="4"/>
+        <f>H55+D56</f>
         <v>26994</v>
       </c>
       <c r="I56">
@@ -2508,19 +2508,19 @@
         <v>168</v>
       </c>
       <c r="Q56" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I56+K56=B56,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R56" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S56" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M56+O56=B56,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T56" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2535,16 +2535,16 @@
         <v>7</v>
       </c>
       <c r="E57" s="4">
-        <f t="shared" si="1"/>
+        <f>B57/D57</f>
         <v>0.14285714285714285</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="7">
-        <f t="shared" si="2"/>
+        <f>B57+G56</f>
         <v>4051</v>
       </c>
       <c r="H57">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>27001</v>
       </c>
       <c r="I57">
@@ -2572,19 +2572,19 @@
         <v>4</v>
       </c>
       <c r="Q57" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I57+K57=B57,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R57" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S57" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M57+O57=B57,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T57" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2599,16 +2599,16 @@
         <v>278</v>
       </c>
       <c r="E58" s="4">
-        <f t="shared" si="1"/>
+        <f>B58/D58</f>
         <v>1.4388489208633094E-2</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="7">
-        <f t="shared" si="2"/>
+        <f>B58+G57</f>
         <v>4055</v>
       </c>
       <c r="H58">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>27279</v>
       </c>
       <c r="I58">
@@ -2636,19 +2636,19 @@
         <v>85</v>
       </c>
       <c r="Q58" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I58+K58=B58,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R58" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S58" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M58+O58=B58,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T58" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2663,16 +2663,16 @@
         <v>1957</v>
       </c>
       <c r="E59" s="4">
-        <f t="shared" si="1"/>
+        <f>B59/D59</f>
         <v>2.6060296371997957E-2</v>
       </c>
       <c r="F59" s="4"/>
       <c r="G59" s="7">
-        <f t="shared" si="2"/>
+        <f>B59+G58</f>
         <v>4106</v>
       </c>
       <c r="H59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>29236</v>
       </c>
       <c r="I59">
@@ -2700,19 +2700,19 @@
         <v>404</v>
       </c>
       <c r="Q59" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I59+K59=B59,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R59" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S59" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M59+O59=B59,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T59" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2727,16 +2727,16 @@
         <v>1908</v>
       </c>
       <c r="E60" s="4">
-        <f t="shared" si="1"/>
+        <f>B60/D60</f>
         <v>1.8343815513626835E-2</v>
       </c>
       <c r="F60" s="4"/>
       <c r="G60" s="7">
-        <f t="shared" si="2"/>
+        <f>B60+G59</f>
         <v>4141</v>
       </c>
       <c r="H60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>31144</v>
       </c>
       <c r="I60">
@@ -2764,19 +2764,19 @@
         <v>238</v>
       </c>
       <c r="Q60" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I60+K60=B60,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R60" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S60" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M60+O60=B60,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T60" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2791,16 +2791,16 @@
         <v>2703</v>
       </c>
       <c r="E61" s="4">
-        <f t="shared" si="1"/>
+        <f>B61/D61</f>
         <v>1.2948575656677765E-2</v>
       </c>
       <c r="F61" s="4"/>
       <c r="G61" s="7">
-        <f t="shared" si="2"/>
+        <f>B61+G60</f>
         <v>4176</v>
       </c>
       <c r="H61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>33847</v>
       </c>
       <c r="I61">
@@ -2828,19 +2828,19 @@
         <v>228</v>
       </c>
       <c r="Q61" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I61+K61=B61,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R61" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S61" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M61+O61=B61,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T61" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2855,16 +2855,16 @@
         <v>1922</v>
       </c>
       <c r="E62" s="4">
-        <f t="shared" si="1"/>
+        <f>B62/D62</f>
         <v>4.6826222684703432E-3</v>
       </c>
       <c r="F62" s="4"/>
       <c r="G62" s="7">
-        <f t="shared" si="2"/>
+        <f>B62+G61</f>
         <v>4185</v>
       </c>
       <c r="H62">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>35769</v>
       </c>
       <c r="I62">
@@ -2892,19 +2892,19 @@
         <v>212</v>
       </c>
       <c r="Q62" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I62+K62=B62,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R62" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S62" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M62+O62=B62,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T62" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2919,16 +2919,16 @@
         <v>1524</v>
       </c>
       <c r="E63" s="4">
-        <f t="shared" si="1"/>
+        <f>B63/D63</f>
         <v>1.1154855643044619E-2</v>
       </c>
       <c r="F63" s="4"/>
       <c r="G63" s="7">
-        <f t="shared" si="2"/>
+        <f>B63+G62</f>
         <v>4202</v>
       </c>
       <c r="H63">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>37293</v>
       </c>
       <c r="I63">
@@ -2956,19 +2956,19 @@
         <v>287</v>
       </c>
       <c r="Q63" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I63+K63=B63,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R63" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S63" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(M63+O63=B63,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T63" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2983,16 +2983,16 @@
         <v>103</v>
       </c>
       <c r="E64" s="4">
-        <f t="shared" si="1"/>
+        <f>B64/D64</f>
         <v>0</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="7">
-        <f t="shared" si="2"/>
+        <f>B64+G63</f>
         <v>4202</v>
       </c>
       <c r="H64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>37396</v>
       </c>
       <c r="I64">
@@ -3020,11 +3020,11 @@
         <v>29</v>
       </c>
       <c r="Q64" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(I64+K64=B64,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R64" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="S64" t="str">
@@ -3032,7 +3032,7 @@
         <v>EQUAL</v>
       </c>
       <c r="T64" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -3332,7 +3332,7 @@
         <v>277</v>
       </c>
       <c r="G4" s="4">
-        <f t="shared" ref="G3:G23" si="0">D4/F4</f>
+        <f t="shared" ref="G4:G23" si="0">D4/F4</f>
         <v>0.3140794223826715</v>
       </c>
       <c r="H4" s="13"/>

</xml_diff>

<commit_message>
Updated data for 10-30-2020 COVID dashboard update
</commit_message>
<xml_diff>
--- a/clemsonDashboard.xlsx
+++ b/clemsonDashboard.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidferrara/Documents/Clemson/The Tiger/COVID-19/Data/ttn-clemson-covid-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AC0A9D-7180-564A-BCCF-9BF51BA288A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62EEDB0-2955-D445-B88B-ADB1CB329AE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16260" xr2:uid="{663FE1B6-0B7E-E04A-924C-6AB15F4F5852}"/>
+    <workbookView xWindow="360" yWindow="460" windowWidth="28040" windowHeight="16260" activeTab="1" xr2:uid="{663FE1B6-0B7E-E04A-924C-6AB15F4F5852}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Data" sheetId="1" r:id="rId1"/>
     <sheet name="Weekly Data" sheetId="4" r:id="rId2"/>
     <sheet name="Isolation and Quarantine" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'Isolation and Quarantine'!$D$2:$D$11</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Isolation and Quarantine'!$D$2:$D$11</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -261,7 +265,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -286,6 +290,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -300,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -339,6 +349,12 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2018E299-360B-F244-BDDD-9B449D0B7C0F}">
   <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -825,7 +841,7 @@
         <v>14</v>
       </c>
       <c r="G3" s="7">
-        <f>B3+G2</f>
+        <f t="shared" ref="G3:G34" si="0">B3+G2</f>
         <v>16</v>
       </c>
       <c r="V3" s="9" t="s">
@@ -840,7 +856,7 @@
         <v>22</v>
       </c>
       <c r="G4" s="7">
-        <f>B4+G3</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
     </row>
@@ -852,7 +868,7 @@
         <v>38</v>
       </c>
       <c r="G5" s="7">
-        <f>B5+G4</f>
+        <f t="shared" si="0"/>
         <v>76</v>
       </c>
     </row>
@@ -864,7 +880,7 @@
         <v>33</v>
       </c>
       <c r="G6" s="7">
-        <f>B6+G5</f>
+        <f t="shared" si="0"/>
         <v>109</v>
       </c>
     </row>
@@ -876,7 +892,7 @@
         <v>46</v>
       </c>
       <c r="G7" s="7">
-        <f>B7+G6</f>
+        <f t="shared" si="0"/>
         <v>155</v>
       </c>
     </row>
@@ -888,7 +904,7 @@
         <v>8</v>
       </c>
       <c r="G8" s="7">
-        <f>B8+G7</f>
+        <f t="shared" si="0"/>
         <v>163</v>
       </c>
     </row>
@@ -900,7 +916,7 @@
         <v>13</v>
       </c>
       <c r="G9" s="7">
-        <f>B9+G8</f>
+        <f t="shared" si="0"/>
         <v>176</v>
       </c>
     </row>
@@ -912,7 +928,7 @@
         <v>108</v>
       </c>
       <c r="G10" s="7">
-        <f>B10+G9</f>
+        <f t="shared" si="0"/>
         <v>284</v>
       </c>
     </row>
@@ -924,7 +940,7 @@
         <v>196</v>
       </c>
       <c r="G11" s="7">
-        <f>B11+G10</f>
+        <f t="shared" si="0"/>
         <v>480</v>
       </c>
     </row>
@@ -936,7 +952,7 @@
         <v>174</v>
       </c>
       <c r="G12" s="7">
-        <f>B12+G11</f>
+        <f t="shared" si="0"/>
         <v>654</v>
       </c>
     </row>
@@ -948,7 +964,7 @@
         <v>198</v>
       </c>
       <c r="G13" s="7">
-        <f>B13+G12</f>
+        <f t="shared" si="0"/>
         <v>852</v>
       </c>
     </row>
@@ -960,7 +976,7 @@
         <v>117</v>
       </c>
       <c r="G14" s="7">
-        <f>B14+G13</f>
+        <f t="shared" si="0"/>
         <v>969</v>
       </c>
     </row>
@@ -972,7 +988,7 @@
         <v>15</v>
       </c>
       <c r="G15" s="7">
-        <f>B15+G14</f>
+        <f t="shared" si="0"/>
         <v>984</v>
       </c>
     </row>
@@ -984,7 +1000,7 @@
         <v>34</v>
       </c>
       <c r="G16" s="7">
-        <f>B16+G15</f>
+        <f t="shared" si="0"/>
         <v>1018</v>
       </c>
     </row>
@@ -996,7 +1012,7 @@
         <v>111</v>
       </c>
       <c r="G17" s="7">
-        <f>B17+G16</f>
+        <f t="shared" si="0"/>
         <v>1129</v>
       </c>
     </row>
@@ -1008,7 +1024,7 @@
         <v>129</v>
       </c>
       <c r="G18" s="7">
-        <f>B18+G17</f>
+        <f t="shared" si="0"/>
         <v>1258</v>
       </c>
     </row>
@@ -1020,7 +1036,7 @@
         <v>103</v>
       </c>
       <c r="G19" s="7">
-        <f>B19+G18</f>
+        <f t="shared" si="0"/>
         <v>1361</v>
       </c>
     </row>
@@ -1032,7 +1048,7 @@
         <v>42</v>
       </c>
       <c r="G20" s="7">
-        <f>B20+G19</f>
+        <f t="shared" si="0"/>
         <v>1403</v>
       </c>
     </row>
@@ -1044,7 +1060,7 @@
         <v>51</v>
       </c>
       <c r="G21" s="7">
-        <f>B21+G20</f>
+        <f t="shared" si="0"/>
         <v>1454</v>
       </c>
     </row>
@@ -1059,7 +1075,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="7">
-        <f>B22+G21</f>
+        <f t="shared" si="0"/>
         <v>1472</v>
       </c>
       <c r="H22" s="3"/>
@@ -1084,7 +1100,7 @@
         <v>34</v>
       </c>
       <c r="G23" s="7">
-        <f>B23+G22</f>
+        <f t="shared" si="0"/>
         <v>1506</v>
       </c>
     </row>
@@ -1096,7 +1112,7 @@
         <v>171</v>
       </c>
       <c r="G24" s="7">
-        <f>B24+G23</f>
+        <f t="shared" si="0"/>
         <v>1677</v>
       </c>
     </row>
@@ -1108,7 +1124,7 @@
         <v>261</v>
       </c>
       <c r="G25" s="7">
-        <f>B25+G24</f>
+        <f t="shared" si="0"/>
         <v>1938</v>
       </c>
     </row>
@@ -1120,7 +1136,7 @@
         <v>183</v>
       </c>
       <c r="G26" s="7">
-        <f>B26+G25</f>
+        <f t="shared" si="0"/>
         <v>2121</v>
       </c>
     </row>
@@ -1132,7 +1148,7 @@
         <v>122</v>
       </c>
       <c r="G27" s="7">
-        <f>B27+G26</f>
+        <f t="shared" si="0"/>
         <v>2243</v>
       </c>
     </row>
@@ -1144,7 +1160,7 @@
         <v>82</v>
       </c>
       <c r="G28" s="7">
-        <f>B28+G27</f>
+        <f t="shared" si="0"/>
         <v>2325</v>
       </c>
     </row>
@@ -1156,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="7">
-        <f>B29+G28</f>
+        <f t="shared" si="0"/>
         <v>2326</v>
       </c>
     </row>
@@ -1168,7 +1184,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="7">
-        <f>B30+G29</f>
+        <f t="shared" si="0"/>
         <v>2329</v>
       </c>
     </row>
@@ -1180,7 +1196,7 @@
         <v>93</v>
       </c>
       <c r="G31" s="7">
-        <f>B31+G30</f>
+        <f t="shared" si="0"/>
         <v>2422</v>
       </c>
     </row>
@@ -1192,7 +1208,7 @@
         <v>34</v>
       </c>
       <c r="G32" s="7">
-        <f>B32+G31</f>
+        <f t="shared" si="0"/>
         <v>2456</v>
       </c>
     </row>
@@ -1204,7 +1220,7 @@
         <v>73</v>
       </c>
       <c r="G33" s="7">
-        <f>B33+G32</f>
+        <f t="shared" si="0"/>
         <v>2529</v>
       </c>
     </row>
@@ -1216,7 +1232,7 @@
         <v>116</v>
       </c>
       <c r="G34" s="7">
-        <f>B34+G33</f>
+        <f t="shared" si="0"/>
         <v>2645</v>
       </c>
     </row>
@@ -1228,7 +1244,7 @@
         <v>92</v>
       </c>
       <c r="G35" s="7">
-        <f>B35+G34</f>
+        <f t="shared" ref="G35:G69" si="1">B35+G34</f>
         <v>2737</v>
       </c>
     </row>
@@ -1240,7 +1256,7 @@
         <v>72</v>
       </c>
       <c r="G36" s="7">
-        <f>B36+G35</f>
+        <f t="shared" si="1"/>
         <v>2809</v>
       </c>
     </row>
@@ -1255,12 +1271,12 @@
         <v>401</v>
       </c>
       <c r="E37" s="4">
-        <f>B37/D37</f>
+        <f t="shared" ref="E37:E69" si="2">B37/D37</f>
         <v>2.2443890274314215E-2</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="7">
-        <f>B37+G36</f>
+        <f t="shared" si="1"/>
         <v>2818</v>
       </c>
       <c r="H37">
@@ -1292,7 +1308,7 @@
         <v>112</v>
       </c>
       <c r="Q37" t="str">
-        <f>IF(I37+K37=B37,"EQUAL","DIFFER")</f>
+        <f t="shared" ref="Q37:Q69" si="3">IF(I37+K37=B37,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="R37" t="str">
@@ -1300,7 +1316,7 @@
         <v>EQUAL</v>
       </c>
       <c r="S37" t="str">
-        <f>IF(M37+O37=B37,"EQUAL","DIFFER")</f>
+        <f t="shared" ref="S37:S69" si="4">IF(M37+O37=B37,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="T37" t="str">
@@ -1319,16 +1335,16 @@
         <v>2170</v>
       </c>
       <c r="E38" s="4">
-        <f>B38/D38</f>
+        <f t="shared" si="2"/>
         <v>8.4792626728110596E-2</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="7">
-        <f>B38+G37</f>
+        <f t="shared" si="1"/>
         <v>3002</v>
       </c>
       <c r="H38">
-        <f t="shared" ref="H38:H64" si="0">H37+D38</f>
+        <f t="shared" ref="H38:H69" si="5">H37+D38</f>
         <v>2571</v>
       </c>
       <c r="I38">
@@ -1356,19 +1372,19 @@
         <v>45</v>
       </c>
       <c r="Q38" t="str">
-        <f>IF(I38+K38=B38,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R38" t="str">
-        <f t="shared" ref="R38:R64" si="1">IF(J38+L38=D38,"EQUAL","DIFFER")</f>
+        <f t="shared" ref="R38:R69" si="6">IF(J38+L38=D38,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="S38" t="str">
-        <f>IF(M38+O38=B38,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T38" t="str">
-        <f t="shared" ref="T38:T64" si="2">IF(N38+P38=D38,"EQUAL","DIFFER")</f>
+        <f t="shared" ref="T38:T69" si="7">IF(N38+P38=D38,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
     </row>
@@ -1383,16 +1399,16 @@
         <v>1272</v>
       </c>
       <c r="E39" s="4">
-        <f>B39/D39</f>
+        <f t="shared" si="2"/>
         <v>5.4245283018867926E-2</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="7">
-        <f>B39+G38</f>
+        <f t="shared" si="1"/>
         <v>3071</v>
       </c>
       <c r="H39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>3843</v>
       </c>
       <c r="I39">
@@ -1420,19 +1436,19 @@
         <v>42</v>
       </c>
       <c r="Q39" t="str">
-        <f>IF(I39+K39=B39,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S39" t="str">
-        <f>IF(M39+O39=B39,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -1447,16 +1463,16 @@
         <v>2062</v>
       </c>
       <c r="E40" s="4">
-        <f>B40/D40</f>
+        <f t="shared" si="2"/>
         <v>7.953443258971872E-2</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="7">
-        <f>B40+G39</f>
+        <f t="shared" si="1"/>
         <v>3235</v>
       </c>
       <c r="H40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>5905</v>
       </c>
       <c r="I40">
@@ -1484,19 +1500,19 @@
         <v>169</v>
       </c>
       <c r="Q40" t="str">
-        <f>IF(I40+K40=B40,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S40" t="str">
-        <f>IF(M40+O40=B40,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -1511,16 +1527,16 @@
         <v>1210</v>
       </c>
       <c r="E41" s="4">
-        <f>B41/D41</f>
+        <f t="shared" si="2"/>
         <v>7.1074380165289261E-2</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="7">
-        <f>B41+G40</f>
+        <f t="shared" si="1"/>
         <v>3321</v>
       </c>
       <c r="H41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7115</v>
       </c>
       <c r="I41">
@@ -1548,19 +1564,19 @@
         <v>37</v>
       </c>
       <c r="Q41" t="str">
-        <f>IF(I41+K41=B41,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S41" t="str">
-        <f>IF(M41+O41=B41,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T41" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -1575,16 +1591,16 @@
         <v>1618</v>
       </c>
       <c r="E42" s="4">
-        <f>B42/D42</f>
+        <f t="shared" si="2"/>
         <v>4.3263288009888753E-2</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="7">
-        <f>B42+G41</f>
+        <f t="shared" si="1"/>
         <v>3391</v>
       </c>
       <c r="H42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>8733</v>
       </c>
       <c r="I42">
@@ -1612,19 +1628,19 @@
         <v>279</v>
       </c>
       <c r="Q42" t="str">
-        <f>IF(I42+K42=B42,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S42" t="str">
-        <f>IF(M42+O42=B42,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -1639,16 +1655,16 @@
         <v>20</v>
       </c>
       <c r="E43" s="4">
-        <f>B43/D43</f>
+        <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="7">
-        <f>B43+G42</f>
+        <f t="shared" si="1"/>
         <v>3397</v>
       </c>
       <c r="H43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>8753</v>
       </c>
       <c r="I43">
@@ -1676,19 +1692,19 @@
         <v>1</v>
       </c>
       <c r="Q43" t="str">
-        <f>IF(I43+K43=B43,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S43" t="str">
-        <f>IF(M43+O43=B43,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -1703,16 +1719,16 @@
         <v>309</v>
       </c>
       <c r="E44" s="4">
-        <f>B44/D44</f>
+        <f t="shared" si="2"/>
         <v>1.2944983818770227E-2</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="7">
-        <f>B44+G43</f>
+        <f t="shared" si="1"/>
         <v>3401</v>
       </c>
       <c r="H44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>9062</v>
       </c>
       <c r="I44">
@@ -1740,19 +1756,19 @@
         <v>99</v>
       </c>
       <c r="Q44" t="str">
-        <f>IF(I44+K44=B44,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S44" t="str">
-        <f>IF(M44+O44=B44,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T44" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -1767,16 +1783,16 @@
         <v>1716</v>
       </c>
       <c r="E45" s="4">
-        <f>B45/D45</f>
+        <f t="shared" si="2"/>
         <v>5.7109557109557112E-2</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="7">
-        <f>B45+G44</f>
+        <f t="shared" si="1"/>
         <v>3499</v>
       </c>
       <c r="H45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>10778</v>
       </c>
       <c r="I45">
@@ -1804,19 +1820,19 @@
         <v>174</v>
       </c>
       <c r="Q45" t="str">
-        <f>IF(I45+K45=B45,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S45" t="str">
-        <f>IF(M45+O45=B45,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -1831,16 +1847,16 @@
         <v>1251</v>
       </c>
       <c r="E46" s="4">
-        <f>B46/D46</f>
+        <f t="shared" si="2"/>
         <v>6.7146282973621102E-2</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="7">
-        <f>B46+G45</f>
+        <f t="shared" si="1"/>
         <v>3583</v>
       </c>
       <c r="H46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>12029</v>
       </c>
       <c r="I46">
@@ -1868,19 +1884,19 @@
         <v>114</v>
       </c>
       <c r="Q46" t="str">
-        <f>IF(I46+K46=B46,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S46" t="str">
-        <f>IF(M46+O46=B46,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T46" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -1895,16 +1911,16 @@
         <v>2690</v>
       </c>
       <c r="E47" s="4">
-        <f>B47/D47</f>
+        <f t="shared" si="2"/>
         <v>3.1226765799256505E-2</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="7">
-        <f>B47+G46</f>
+        <f t="shared" si="1"/>
         <v>3667</v>
       </c>
       <c r="H47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>14719</v>
       </c>
       <c r="I47">
@@ -1932,19 +1948,19 @@
         <v>454</v>
       </c>
       <c r="Q47" t="str">
-        <f>IF(I47+K47=B47,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S47" t="str">
-        <f>IF(M47+O47=B47,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T47" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -1959,16 +1975,16 @@
         <v>1374</v>
       </c>
       <c r="E48" s="4">
-        <f>B48/D48</f>
+        <f t="shared" si="2"/>
         <v>3.7117903930131008E-2</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="7">
-        <f>B48+G47</f>
+        <f t="shared" si="1"/>
         <v>3718</v>
       </c>
       <c r="H48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>16093</v>
       </c>
       <c r="I48">
@@ -1996,19 +2012,19 @@
         <v>111</v>
       </c>
       <c r="Q48" t="str">
-        <f>IF(I48+K48=B48,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S48" t="str">
-        <f>IF(M48+O48=B48,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T48" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2023,16 +2039,16 @@
         <v>1601</v>
       </c>
       <c r="E49" s="4">
-        <f>B49/D49</f>
+        <f t="shared" si="2"/>
         <v>4.996876951905059E-2</v>
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="7">
-        <f>B49+G48</f>
+        <f t="shared" si="1"/>
         <v>3798</v>
       </c>
       <c r="H49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>17694</v>
       </c>
       <c r="I49">
@@ -2060,19 +2076,19 @@
         <v>149</v>
       </c>
       <c r="Q49" t="str">
-        <f>IF(I49+K49=B49,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R49" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S49" t="str">
-        <f>IF(M49+O49=B49,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T49" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2087,16 +2103,16 @@
         <v>282</v>
       </c>
       <c r="E50" s="4">
-        <f>B50/D50</f>
+        <f t="shared" si="2"/>
         <v>2.1276595744680851E-2</v>
       </c>
       <c r="F50" s="4"/>
       <c r="G50" s="7">
-        <f>B50+G49</f>
+        <f t="shared" si="1"/>
         <v>3804</v>
       </c>
       <c r="H50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>17976</v>
       </c>
       <c r="I50">
@@ -2124,19 +2140,19 @@
         <v>66</v>
       </c>
       <c r="Q50" t="str">
-        <f>IF(I50+K50=B50,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S50" t="str">
-        <f>IF(M50+O50=B50,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2151,16 +2167,16 @@
         <v>270</v>
       </c>
       <c r="E51" s="4">
-        <f>B51/D51</f>
+        <f t="shared" si="2"/>
         <v>1.8518518518518517E-2</v>
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="7">
-        <f>B51+G50</f>
+        <f t="shared" si="1"/>
         <v>3809</v>
       </c>
       <c r="H51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>18246</v>
       </c>
       <c r="I51">
@@ -2188,19 +2204,19 @@
         <v>90</v>
       </c>
       <c r="Q51" t="str">
-        <f>IF(I51+K51=B51,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S51" t="str">
-        <f>IF(M51+O51=B51,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T51" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2215,16 +2231,16 @@
         <v>1606</v>
       </c>
       <c r="E52" s="4">
-        <f>B52/D52</f>
+        <f t="shared" si="2"/>
         <v>5.7285180572851806E-2</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="7">
-        <f>B52+G51</f>
+        <f t="shared" si="1"/>
         <v>3901</v>
       </c>
       <c r="H52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>19852</v>
       </c>
       <c r="I52">
@@ -2252,19 +2268,19 @@
         <v>247</v>
       </c>
       <c r="Q52" t="str">
-        <f>IF(I52+K52=B52,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S52" t="str">
-        <f>IF(M52+O52=B52,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T52" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2279,16 +2295,16 @@
         <v>1714</v>
       </c>
       <c r="E53" s="4">
-        <f>B53/D53</f>
+        <f t="shared" si="2"/>
         <v>2.8588098016336057E-2</v>
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="7">
-        <f>B53+G52</f>
+        <f t="shared" si="1"/>
         <v>3950</v>
       </c>
       <c r="H53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>21566</v>
       </c>
       <c r="I53">
@@ -2316,19 +2332,19 @@
         <v>122</v>
       </c>
       <c r="Q53" t="str">
-        <f>IF(I53+K53=B53,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R53" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S53" t="str">
-        <f>IF(M53+O53=B53,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T53" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2343,16 +2359,16 @@
         <v>2925</v>
       </c>
       <c r="E54" s="4">
-        <f>B54/D54</f>
+        <f t="shared" si="2"/>
         <v>1.5726495726495728E-2</v>
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="7">
-        <f>B54+G53</f>
+        <f t="shared" si="1"/>
         <v>3996</v>
       </c>
       <c r="H54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>24491</v>
       </c>
       <c r="I54">
@@ -2380,19 +2396,19 @@
         <v>348</v>
       </c>
       <c r="Q54" t="str">
-        <f>IF(I54+K54=B54,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R54" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S54" t="str">
-        <f>IF(M54+O54=B54,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T54" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2407,16 +2423,16 @@
         <v>1690</v>
       </c>
       <c r="E55" s="4">
-        <f>B55/D55</f>
+        <f t="shared" si="2"/>
         <v>1.242603550295858E-2</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="7">
-        <f>B55+G54</f>
+        <f t="shared" si="1"/>
         <v>4017</v>
       </c>
       <c r="H55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>26181</v>
       </c>
       <c r="I55">
@@ -2444,19 +2460,19 @@
         <v>75</v>
       </c>
       <c r="Q55" t="str">
-        <f>IF(I55+K55=B55,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R55" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S55" t="str">
-        <f>IF(M55+O55=B55,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T55" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2471,12 +2487,12 @@
         <v>813</v>
       </c>
       <c r="E56" s="4">
-        <f>B56/D56</f>
+        <f t="shared" si="2"/>
         <v>4.0590405904059039E-2</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="7">
-        <f>B56+G55</f>
+        <f t="shared" si="1"/>
         <v>4050</v>
       </c>
       <c r="H56">
@@ -2508,19 +2524,19 @@
         <v>168</v>
       </c>
       <c r="Q56" t="str">
-        <f>IF(I56+K56=B56,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R56" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S56" t="str">
-        <f>IF(M56+O56=B56,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T56" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2535,16 +2551,16 @@
         <v>7</v>
       </c>
       <c r="E57" s="4">
-        <f>B57/D57</f>
+        <f t="shared" si="2"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="7">
-        <f>B57+G56</f>
+        <f t="shared" si="1"/>
         <v>4051</v>
       </c>
       <c r="H57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>27001</v>
       </c>
       <c r="I57">
@@ -2572,19 +2588,19 @@
         <v>4</v>
       </c>
       <c r="Q57" t="str">
-        <f>IF(I57+K57=B57,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R57" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S57" t="str">
-        <f>IF(M57+O57=B57,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T57" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2599,16 +2615,16 @@
         <v>278</v>
       </c>
       <c r="E58" s="4">
-        <f>B58/D58</f>
+        <f t="shared" si="2"/>
         <v>1.4388489208633094E-2</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="7">
-        <f>B58+G57</f>
+        <f t="shared" si="1"/>
         <v>4055</v>
       </c>
       <c r="H58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>27279</v>
       </c>
       <c r="I58">
@@ -2636,19 +2652,19 @@
         <v>85</v>
       </c>
       <c r="Q58" t="str">
-        <f>IF(I58+K58=B58,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S58" t="str">
-        <f>IF(M58+O58=B58,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T58" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2663,16 +2679,16 @@
         <v>1957</v>
       </c>
       <c r="E59" s="4">
-        <f>B59/D59</f>
+        <f t="shared" si="2"/>
         <v>2.6060296371997957E-2</v>
       </c>
       <c r="F59" s="4"/>
       <c r="G59" s="7">
-        <f>B59+G58</f>
+        <f t="shared" si="1"/>
         <v>4106</v>
       </c>
       <c r="H59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>29236</v>
       </c>
       <c r="I59">
@@ -2700,19 +2716,19 @@
         <v>404</v>
       </c>
       <c r="Q59" t="str">
-        <f>IF(I59+K59=B59,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R59" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S59" t="str">
-        <f>IF(M59+O59=B59,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T59" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2727,16 +2743,16 @@
         <v>1908</v>
       </c>
       <c r="E60" s="4">
-        <f>B60/D60</f>
+        <f t="shared" si="2"/>
         <v>1.8343815513626835E-2</v>
       </c>
       <c r="F60" s="4"/>
       <c r="G60" s="7">
-        <f>B60+G59</f>
+        <f t="shared" si="1"/>
         <v>4141</v>
       </c>
       <c r="H60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>31144</v>
       </c>
       <c r="I60">
@@ -2764,19 +2780,19 @@
         <v>238</v>
       </c>
       <c r="Q60" t="str">
-        <f>IF(I60+K60=B60,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R60" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S60" t="str">
-        <f>IF(M60+O60=B60,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T60" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2791,16 +2807,16 @@
         <v>2703</v>
       </c>
       <c r="E61" s="4">
-        <f>B61/D61</f>
+        <f t="shared" si="2"/>
         <v>1.2948575656677765E-2</v>
       </c>
       <c r="F61" s="4"/>
       <c r="G61" s="7">
-        <f>B61+G60</f>
+        <f t="shared" si="1"/>
         <v>4176</v>
       </c>
       <c r="H61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>33847</v>
       </c>
       <c r="I61">
@@ -2828,19 +2844,19 @@
         <v>228</v>
       </c>
       <c r="Q61" t="str">
-        <f>IF(I61+K61=B61,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R61" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S61" t="str">
-        <f>IF(M61+O61=B61,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T61" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2855,16 +2871,16 @@
         <v>1922</v>
       </c>
       <c r="E62" s="4">
-        <f>B62/D62</f>
+        <f t="shared" si="2"/>
         <v>4.6826222684703432E-3</v>
       </c>
       <c r="F62" s="4"/>
       <c r="G62" s="7">
-        <f>B62+G61</f>
+        <f t="shared" si="1"/>
         <v>4185</v>
       </c>
       <c r="H62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>35769</v>
       </c>
       <c r="I62">
@@ -2892,19 +2908,19 @@
         <v>212</v>
       </c>
       <c r="Q62" t="str">
-        <f>IF(I62+K62=B62,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R62" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S62" t="str">
-        <f>IF(M62+O62=B62,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T62" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2919,16 +2935,16 @@
         <v>1524</v>
       </c>
       <c r="E63" s="4">
-        <f>B63/D63</f>
+        <f t="shared" si="2"/>
         <v>1.1154855643044619E-2</v>
       </c>
       <c r="F63" s="4"/>
       <c r="G63" s="7">
-        <f>B63+G62</f>
+        <f t="shared" si="1"/>
         <v>4202</v>
       </c>
       <c r="H63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>37293</v>
       </c>
       <c r="I63">
@@ -2956,19 +2972,19 @@
         <v>287</v>
       </c>
       <c r="Q63" t="str">
-        <f>IF(I63+K63=B63,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R63" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S63" t="str">
-        <f>IF(M63+O63=B63,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T63" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -2983,16 +2999,16 @@
         <v>103</v>
       </c>
       <c r="E64" s="4">
-        <f>B64/D64</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="7">
-        <f>B64+G63</f>
+        <f t="shared" si="1"/>
         <v>4202</v>
       </c>
       <c r="H64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>37396</v>
       </c>
       <c r="I64">
@@ -3020,62 +3036,347 @@
         <v>29</v>
       </c>
       <c r="Q64" t="str">
-        <f>IF(I64+K64=B64,"EQUAL","DIFFER")</f>
+        <f t="shared" si="3"/>
         <v>EQUAL</v>
       </c>
       <c r="R64" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>EQUAL</v>
       </c>
       <c r="S64" t="str">
-        <f>IF(M64+O64=B64,"EQUAL","DIFFER")</f>
+        <f t="shared" si="4"/>
         <v>EQUAL</v>
       </c>
       <c r="T64" t="str">
-        <f t="shared" si="2"/>
-        <v>EQUAL</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
+        <f t="shared" si="7"/>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20">
       <c r="A65" s="6">
         <v>44129</v>
       </c>
-      <c r="E65" s="4"/>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>270</v>
+      </c>
+      <c r="E65" s="4">
+        <f t="shared" si="2"/>
+        <v>3.7037037037037038E-3</v>
+      </c>
       <c r="F65" s="4"/>
-      <c r="G65" s="7"/>
-    </row>
-    <row r="66" spans="1:7">
+      <c r="G65" s="7">
+        <f t="shared" si="1"/>
+        <v>4203</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="5"/>
+        <v>37666</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>1</v>
+      </c>
+      <c r="L65">
+        <v>270</v>
+      </c>
+      <c r="M65">
+        <v>1</v>
+      </c>
+      <c r="N65">
+        <v>183</v>
+      </c>
+      <c r="O65">
+        <v>0</v>
+      </c>
+      <c r="P65">
+        <v>87</v>
+      </c>
+      <c r="Q65" t="str">
+        <f t="shared" si="3"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="R65" t="str">
+        <f t="shared" si="6"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="S65" t="str">
+        <f t="shared" si="4"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="T65" t="str">
+        <f t="shared" si="7"/>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20">
       <c r="A66" s="6">
         <v>44130</v>
       </c>
-      <c r="E66" s="4"/>
+      <c r="B66">
+        <v>17</v>
+      </c>
+      <c r="D66">
+        <v>2248</v>
+      </c>
+      <c r="E66" s="4">
+        <f t="shared" si="2"/>
+        <v>7.5622775800711743E-3</v>
+      </c>
       <c r="F66" s="4"/>
-      <c r="G66" s="7"/>
-    </row>
-    <row r="67" spans="1:7">
+      <c r="G66" s="7">
+        <f t="shared" si="1"/>
+        <v>4220</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="5"/>
+        <v>39914</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>5</v>
+      </c>
+      <c r="K66">
+        <v>17</v>
+      </c>
+      <c r="L66">
+        <v>2243</v>
+      </c>
+      <c r="M66">
+        <v>14</v>
+      </c>
+      <c r="N66">
+        <v>1825</v>
+      </c>
+      <c r="O66">
+        <v>3</v>
+      </c>
+      <c r="P66">
+        <v>423</v>
+      </c>
+      <c r="Q66" t="str">
+        <f t="shared" si="3"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="R66" t="str">
+        <f t="shared" si="6"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="S66" t="str">
+        <f t="shared" si="4"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="T66" t="str">
+        <f t="shared" si="7"/>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20">
       <c r="A67" s="6">
         <v>44131</v>
       </c>
-      <c r="E67" s="4"/>
+      <c r="B67">
+        <v>19</v>
+      </c>
+      <c r="D67">
+        <v>2020</v>
+      </c>
+      <c r="E67" s="4">
+        <f t="shared" si="2"/>
+        <v>9.4059405940594056E-3</v>
+      </c>
       <c r="F67" s="4"/>
-      <c r="G67" s="7"/>
-    </row>
-    <row r="68" spans="1:7">
+      <c r="G67" s="7">
+        <f t="shared" si="1"/>
+        <v>4239</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="5"/>
+        <v>41934</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>8</v>
+      </c>
+      <c r="K67">
+        <v>19</v>
+      </c>
+      <c r="L67">
+        <v>2012</v>
+      </c>
+      <c r="M67">
+        <v>19</v>
+      </c>
+      <c r="N67">
+        <v>1849</v>
+      </c>
+      <c r="O67">
+        <v>0</v>
+      </c>
+      <c r="P67">
+        <v>171</v>
+      </c>
+      <c r="Q67" t="str">
+        <f t="shared" si="3"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="R67" t="str">
+        <f t="shared" si="6"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="S67" t="str">
+        <f t="shared" si="4"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="T67" t="str">
+        <f t="shared" si="7"/>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20">
       <c r="A68" s="6">
         <v>44132</v>
       </c>
-    </row>
-    <row r="69" spans="1:7">
+      <c r="B68">
+        <v>23</v>
+      </c>
+      <c r="D68">
+        <v>2839</v>
+      </c>
+      <c r="E68" s="4">
+        <f t="shared" si="2"/>
+        <v>8.1014441704825649E-3</v>
+      </c>
+      <c r="G68" s="7">
+        <f t="shared" si="1"/>
+        <v>4262</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="5"/>
+        <v>44773</v>
+      </c>
+      <c r="I68">
+        <v>1</v>
+      </c>
+      <c r="J68">
+        <v>14</v>
+      </c>
+      <c r="K68">
+        <v>22</v>
+      </c>
+      <c r="L68">
+        <v>2825</v>
+      </c>
+      <c r="M68">
+        <v>22</v>
+      </c>
+      <c r="N68">
+        <v>2370</v>
+      </c>
+      <c r="O68">
+        <v>1</v>
+      </c>
+      <c r="P68">
+        <v>469</v>
+      </c>
+      <c r="Q68" t="str">
+        <f t="shared" si="3"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="R68" t="str">
+        <f t="shared" si="6"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="S68" t="str">
+        <f t="shared" si="4"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="T68" t="str">
+        <f t="shared" si="7"/>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20">
       <c r="A69" s="6">
         <v>44133</v>
       </c>
-    </row>
-    <row r="70" spans="1:7">
+      <c r="B69">
+        <v>3</v>
+      </c>
+      <c r="D69">
+        <v>7</v>
+      </c>
+      <c r="E69" s="4">
+        <f t="shared" si="2"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="G69" s="7">
+        <f t="shared" si="1"/>
+        <v>4265</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="5"/>
+        <v>44780</v>
+      </c>
+      <c r="I69">
+        <v>3</v>
+      </c>
+      <c r="J69">
+        <v>6</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <v>1</v>
+      </c>
+      <c r="M69">
+        <v>3</v>
+      </c>
+      <c r="N69">
+        <v>7</v>
+      </c>
+      <c r="O69">
+        <v>0</v>
+      </c>
+      <c r="P69">
+        <v>0</v>
+      </c>
+      <c r="Q69" t="str">
+        <f t="shared" si="3"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="R69" t="str">
+        <f t="shared" si="6"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="S69" t="str">
+        <f t="shared" si="4"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="T69" t="str">
+        <f t="shared" si="7"/>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20">
       <c r="A70" s="6">
         <v>44134</v>
       </c>
-    </row>
-    <row r="71" spans="1:7">
+      <c r="G70" s="7"/>
+    </row>
+    <row r="71" spans="1:20">
       <c r="A71" s="6">
         <v>44135</v>
       </c>
@@ -3097,8 +3398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D56922A-034D-7E4D-80AB-A29316427207}">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3106,7 +3407,10 @@
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="3.1640625" customWidth="1"/>
     <col min="3" max="3" width="8.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.6640625" customWidth="1"/>
     <col min="9" max="9" width="20.33203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="19.83203125" customWidth="1"/>
@@ -3361,7 +3665,7 @@
         <v>DIFFER</v>
       </c>
       <c r="T4" t="str">
-        <f t="shared" ref="T4:T19" si="4">IF(L4+N4=F4,"EQUAL","DIFFER")</f>
+        <f t="shared" ref="T4:T23" si="4">IF(L4+N4=F4,"EQUAL","DIFFER")</f>
         <v>DIFFER</v>
       </c>
       <c r="U4" t="str">
@@ -4193,18 +4497,28 @@
       <c r="C20" s="20">
         <v>44114</v>
       </c>
-      <c r="G20" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="D20">
+        <v>407</v>
+      </c>
+      <c r="F20" s="9">
+        <v>9224</v>
+      </c>
+      <c r="G20" s="4">
+        <f t="shared" si="0"/>
+        <v>4.4124024284475281E-2</v>
       </c>
       <c r="H20" s="13"/>
       <c r="I20" s="1">
         <f t="shared" si="1"/>
-        <v>3174</v>
+        <v>3581</v>
       </c>
       <c r="J20">
         <f t="shared" si="2"/>
-        <v>56443</v>
+        <v>65667</v>
+      </c>
+      <c r="T20" t="str">
+        <f t="shared" si="4"/>
+        <v>DIFFER</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -4217,18 +4531,28 @@
       <c r="C21" s="20">
         <v>44121</v>
       </c>
-      <c r="G21" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="D21">
+        <v>249</v>
+      </c>
+      <c r="F21" s="9">
+        <v>9032</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" si="0"/>
+        <v>2.7568644818423384E-2</v>
       </c>
       <c r="H21" s="13"/>
       <c r="I21" s="1">
         <f t="shared" si="1"/>
-        <v>3174</v>
+        <v>3830</v>
       </c>
       <c r="J21">
         <f t="shared" si="2"/>
-        <v>56443</v>
+        <v>74699</v>
+      </c>
+      <c r="T21" t="str">
+        <f t="shared" si="4"/>
+        <v>DIFFER</v>
       </c>
     </row>
     <row r="22" spans="1:20">
@@ -4241,18 +4565,28 @@
       <c r="C22" s="20">
         <v>44128</v>
       </c>
-      <c r="G22" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="D22">
+        <v>154</v>
+      </c>
+      <c r="F22" s="9">
+        <v>10423</v>
+      </c>
+      <c r="G22" s="4">
+        <f t="shared" si="0"/>
+        <v>1.4775016789791807E-2</v>
       </c>
       <c r="H22" s="13"/>
       <c r="I22" s="1">
         <f t="shared" si="1"/>
-        <v>3174</v>
+        <v>3984</v>
       </c>
       <c r="J22">
         <f t="shared" si="2"/>
-        <v>56443</v>
+        <v>85122</v>
+      </c>
+      <c r="T22" t="str">
+        <f t="shared" si="4"/>
+        <v>DIFFER</v>
       </c>
     </row>
     <row r="23" spans="1:20">
@@ -4262,21 +4596,31 @@
       <c r="B23" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="20">
-        <v>44135</v>
-      </c>
-      <c r="G23" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="C23" s="24">
+        <v>44133</v>
+      </c>
+      <c r="D23">
+        <v>63</v>
+      </c>
+      <c r="F23" s="9">
+        <v>7384</v>
+      </c>
+      <c r="G23" s="4">
+        <f t="shared" si="0"/>
+        <v>8.5319609967497295E-3</v>
       </c>
       <c r="H23" s="13"/>
       <c r="I23" s="1">
         <f t="shared" si="1"/>
-        <v>3174</v>
+        <v>4047</v>
       </c>
       <c r="J23">
         <f t="shared" si="2"/>
-        <v>56443</v>
+        <v>92506</v>
+      </c>
+      <c r="T23" t="str">
+        <f t="shared" si="4"/>
+        <v>DIFFER</v>
       </c>
     </row>
     <row r="24" spans="1:20">
@@ -4313,15 +4657,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE67BA8-2D94-544F-9655-C971E88AFA0C}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="9" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
   </cols>
@@ -4340,19 +4684,139 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" s="3" customFormat="1">
       <c r="A2" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2">
+        <v>44100</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="27"/>
+      <c r="D3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2">
+        <v>44105</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2">
+        <v>44112</v>
+      </c>
+      <c r="B5" s="9">
+        <v>243</v>
+      </c>
+      <c r="C5">
+        <v>289</v>
+      </c>
+      <c r="D5">
+        <f>B5+C5</f>
+        <v>532</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2">
+        <v>44116</v>
+      </c>
+      <c r="B6" s="9">
+        <v>193</v>
+      </c>
+      <c r="C6">
+        <v>218</v>
+      </c>
+      <c r="D6">
+        <f>B6+C6</f>
+        <v>411</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2">
+        <v>44119</v>
+      </c>
+      <c r="B7" s="9">
+        <v>176</v>
+      </c>
+      <c r="C7">
+        <v>223</v>
+      </c>
+      <c r="D7">
+        <f>B7+C7</f>
+        <v>399</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2">
+        <v>44123</v>
+      </c>
+      <c r="B8" s="9">
+        <v>175</v>
+      </c>
+      <c r="C8">
+        <v>142</v>
+      </c>
+      <c r="D8">
+        <f>B8+C8</f>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="25">
+        <v>44126</v>
+      </c>
+      <c r="B9" s="9">
+        <v>84</v>
+      </c>
+      <c r="C9" s="9">
+        <v>75</v>
+      </c>
+      <c r="D9">
+        <f>B9+C9</f>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2">
         <v>44130</v>
       </c>
-      <c r="B2">
+      <c r="B10" s="9">
         <v>75</v>
       </c>
-      <c r="C2">
+      <c r="C10">
         <v>58</v>
       </c>
-      <c r="D2">
-        <f>B2+C2</f>
+      <c r="D10">
+        <f>B10+C10</f>
         <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2">
+        <v>44133</v>
+      </c>
+      <c r="B11" s="9">
+        <v>51</v>
+      </c>
+      <c r="C11">
+        <v>49</v>
+      </c>
+      <c r="D11">
+        <f>B11+C11</f>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Clemson dashboard with data from EOW Oct 31 up to Nov 2
</commit_message>
<xml_diff>
--- a/clemsonDashboard.xlsx
+++ b/clemsonDashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidferrara/Documents/Clemson/The Tiger/COVID-19/Data/ttn-clemson-covid-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665995EA-FCB2-4744-97FB-86009F74A9DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325C45C1-20E2-CF4C-8F21-715AAFC96190}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="460" windowWidth="28040" windowHeight="16260" activeTab="1" xr2:uid="{663FE1B6-0B7E-E04A-924C-6AB15F4F5852}"/>
+    <workbookView xWindow="340" yWindow="460" windowWidth="28040" windowHeight="16260" xr2:uid="{663FE1B6-0B7E-E04A-924C-6AB15F4F5852}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Data" sheetId="1" r:id="rId1"/>
@@ -419,7 +419,7 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -800,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2018E299-360B-F244-BDDD-9B449D0B7C0F}">
   <dimension ref="A1:X71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1148,7 +1148,7 @@
         <v>13</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:C69" si="2">AVERAGE(B3:B9)</f>
+        <f t="shared" ref="C9:C71" si="2">AVERAGE(B3:B9)</f>
         <v>24.857142857142858</v>
       </c>
       <c r="D9" s="24">
@@ -2122,7 +2122,7 @@
       <c r="G35" s="20"/>
       <c r="H35" s="20"/>
       <c r="I35" s="7">
-        <f t="shared" ref="I35:I69" si="3">B35+I34</f>
+        <f t="shared" ref="I35:I71" si="3">B35+I34</f>
         <v>2737</v>
       </c>
       <c r="J35" s="20"/>
@@ -2199,7 +2199,7 @@
         <v>1552.9393540391914</v>
       </c>
       <c r="G37" s="4">
-        <f t="shared" ref="G37:G69" si="4">B37/E37</f>
+        <f t="shared" ref="G37:G71" si="4">B37/E37</f>
         <v>2.2443890274314215E-2</v>
       </c>
       <c r="H37" s="22"/>
@@ -2271,7 +2271,7 @@
         <v>2170</v>
       </c>
       <c r="F38">
-        <f t="shared" ref="F38:F69" si="7">(E38/25822)*100000</f>
+        <f t="shared" ref="F38:F71" si="7">(E38/25822)*100000</f>
         <v>8403.6867787158244</v>
       </c>
       <c r="G38" s="4">
@@ -2284,7 +2284,7 @@
         <v>3002</v>
       </c>
       <c r="J38">
-        <f t="shared" ref="J38:J69" si="8">J37+E38</f>
+        <f t="shared" ref="J38:J71" si="8">J37+E38</f>
         <v>2571</v>
       </c>
       <c r="K38">
@@ -2738,7 +2738,7 @@
         <v>1.2944983818770227E-2</v>
       </c>
       <c r="H44" s="4">
-        <f t="shared" ref="H44:H69" si="11">AVERAGE(G38:G44)</f>
+        <f t="shared" ref="H44:H71" si="11">AVERAGE(G38:G44)</f>
         <v>9.2264999190092206E-2</v>
       </c>
       <c r="I44" s="7">
@@ -4540,7 +4540,7 @@
         <v>14</v>
       </c>
       <c r="D67" s="24">
-        <f t="shared" ref="D67:D69" si="12">(B67/25822)*100000</f>
+        <f t="shared" ref="D67:D71" si="12">(B67/25822)*100000</f>
         <v>73.580667647742231</v>
       </c>
       <c r="E67">
@@ -4769,11 +4769,110 @@
       <c r="A70" s="6">
         <v>44134</v>
       </c>
-      <c r="I70" s="7"/>
+      <c r="B70">
+        <v>21</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="D70" s="24">
+        <f t="shared" si="12"/>
+        <v>81.326001084346686</v>
+      </c>
+      <c r="E70">
+        <v>2189</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="7"/>
+        <v>8477.2674463635667</v>
+      </c>
+      <c r="G70" s="4">
+        <f t="shared" si="4"/>
+        <v>9.593421653723162E-3</v>
+      </c>
+      <c r="H70" s="4">
+        <f t="shared" si="11"/>
+        <v>6.6705459467638367E-2</v>
+      </c>
+      <c r="I70" s="7">
+        <f t="shared" si="3"/>
+        <v>4286</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="8"/>
+        <v>46969</v>
+      </c>
+      <c r="S70" t="str">
+        <f t="shared" ref="S70:S71" si="13">IF(K70+M70=B70,"EQUAL","DIFFER")</f>
+        <v>DIFFER</v>
+      </c>
+      <c r="T70" t="str">
+        <f t="shared" ref="T70:T71" si="14">IF(L70+N70=E70,"EQUAL","DIFFER")</f>
+        <v>DIFFER</v>
+      </c>
+      <c r="U70" t="str">
+        <f t="shared" ref="U70:U71" si="15">IF(O70+Q70=B70,"EQUAL","DIFFER")</f>
+        <v>DIFFER</v>
+      </c>
+      <c r="V70" t="str">
+        <f t="shared" ref="V70:V71" si="16">IF(P70+R70=E70,"EQUAL","DIFFER")</f>
+        <v>DIFFER</v>
+      </c>
     </row>
     <row r="71" spans="1:22">
       <c r="A71" s="6">
         <v>44135</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="2"/>
+        <v>12.142857142857142</v>
+      </c>
+      <c r="D71" s="24">
+        <f t="shared" si="12"/>
+        <v>3.8726667183022232</v>
+      </c>
+      <c r="E71">
+        <v>2</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="7"/>
+        <v>7.7453334366044464</v>
+      </c>
+      <c r="G71" s="4">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="H71" s="4">
+        <f t="shared" si="11"/>
+        <v>0.13813403089620979</v>
+      </c>
+      <c r="I71" s="7">
+        <f t="shared" si="3"/>
+        <v>4287</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="8"/>
+        <v>46971</v>
+      </c>
+      <c r="S71" t="str">
+        <f t="shared" si="13"/>
+        <v>DIFFER</v>
+      </c>
+      <c r="T71" t="str">
+        <f t="shared" si="14"/>
+        <v>DIFFER</v>
+      </c>
+      <c r="U71" t="str">
+        <f t="shared" si="15"/>
+        <v>DIFFER</v>
+      </c>
+      <c r="V71" t="str">
+        <f t="shared" si="16"/>
+        <v>DIFFER</v>
       </c>
     </row>
   </sheetData>
@@ -4787,7 +4886,7 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="C8:C69" formulaRange="1"/>
+    <ignoredError sqref="C8:C69 C70:C71" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -4796,8 +4895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D56922A-034D-7E4D-80AB-A29316427207}">
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C23"/>
+    <sheetView topLeftCell="J1" zoomScale="95" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4926,7 +5025,7 @@
         <v>158.77933545039113</v>
       </c>
       <c r="I2" s="4">
-        <f>D2/G2</f>
+        <f t="shared" ref="I2:I23" si="0">D2/G2</f>
         <v>2.4390243902439025E-2</v>
       </c>
       <c r="J2" s="23"/>
@@ -4957,11 +5056,11 @@
       <c r="U2" s="20"/>
       <c r="V2" s="20"/>
       <c r="W2" t="str">
-        <f>IF(S2+Q2=D2,"EQUAL","DIFFER")</f>
+        <f t="shared" ref="W2:W23" si="1">IF(S2+Q2=D2,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="X2" t="str">
-        <f>IF(T2+R2=G2,"EQUAL","DIFFER")</f>
+        <f t="shared" ref="X2:X18" si="2">IF(T2+R2=G2,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="Z2" t="s">
@@ -4983,23 +5082,23 @@
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="24">
-        <f t="shared" ref="F3:F23" si="0">(D3/25822)*100000</f>
+        <f t="shared" ref="F3:F23" si="3">(D3/25822)*100000</f>
         <v>15.490666873208893</v>
       </c>
       <c r="G3">
         <v>143</v>
       </c>
       <c r="H3" s="9">
-        <f t="shared" ref="H3:H23" si="1">(G3/25822)*100000</f>
+        <f t="shared" ref="H3:H23" si="4">(G3/25822)*100000</f>
         <v>553.79134071721785</v>
       </c>
       <c r="I3" s="4">
-        <f>D3/G3</f>
+        <f t="shared" si="0"/>
         <v>2.7972027972027972E-2</v>
       </c>
       <c r="J3" s="23"/>
       <c r="K3" s="1">
-        <f>D3+K2</f>
+        <f t="shared" ref="K3:K23" si="5">D3+K2</f>
         <v>5</v>
       </c>
       <c r="L3">
@@ -5025,11 +5124,11 @@
       <c r="U3" s="20"/>
       <c r="V3" s="20"/>
       <c r="W3" t="str">
-        <f>IF(S3+Q3=D3,"EQUAL","DIFFER")</f>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="X3" t="str">
-        <f>IF(T3+R3=G3,"EQUAL","DIFFER")</f>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
       <c r="Z3" t="s">
@@ -5051,27 +5150,27 @@
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>336.92200449229341</v>
       </c>
       <c r="G4">
         <v>277</v>
       </c>
       <c r="H4" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1072.7286809697157</v>
       </c>
       <c r="I4" s="4">
-        <f>D4/G4</f>
+        <f t="shared" si="0"/>
         <v>0.3140794223826715</v>
       </c>
       <c r="J4" s="23"/>
       <c r="K4" s="1">
-        <f>D4+K3</f>
+        <f t="shared" si="5"/>
         <v>92</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L23" si="2">G4+L3</f>
+        <f t="shared" ref="L4:L23" si="6">G4+L3</f>
         <v>461</v>
       </c>
       <c r="M4" s="20"/>
@@ -5093,11 +5192,11 @@
       <c r="U4" s="20"/>
       <c r="V4" s="20"/>
       <c r="W4" t="str">
-        <f>IF(S4+Q4=D4,"EQUAL","DIFFER")</f>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="X4" t="str">
-        <f>IF(T4+R4=G4,"EQUAL","DIFFER")</f>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -5119,18 +5218,18 @@
         <v>34.5</v>
       </c>
       <c r="F5" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>178.14266904190225</v>
       </c>
       <c r="G5">
         <v>298</v>
       </c>
       <c r="H5" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1154.0546820540624</v>
       </c>
       <c r="I5" s="4">
-        <f>D5/G5</f>
+        <f t="shared" si="0"/>
         <v>0.15436241610738255</v>
       </c>
       <c r="J5" s="13">
@@ -5138,11 +5237,11 @@
         <v>0.13020102759113028</v>
       </c>
       <c r="K5" s="1">
-        <f>D5+K4</f>
+        <f t="shared" si="5"/>
         <v>138</v>
       </c>
       <c r="L5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>759</v>
       </c>
       <c r="M5" s="20"/>
@@ -5164,11 +5263,11 @@
       <c r="U5" s="20"/>
       <c r="V5" s="20"/>
       <c r="W5" t="str">
-        <f>IF(S5+Q5=D5,"EQUAL","DIFFER")</f>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="X5" t="str">
-        <f>IF(T5+R5=G5,"EQUAL","DIFFER")</f>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
       <c r="Z5" t="s">
@@ -5189,34 +5288,34 @@
         <v>29</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E23" si="3">AVERAGE(D3:D6)</f>
+        <f t="shared" ref="E6:E23" si="7">AVERAGE(D3:D6)</f>
         <v>41.5</v>
       </c>
       <c r="F6" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>112.30733483076447</v>
       </c>
       <c r="G6">
         <v>149</v>
       </c>
       <c r="H6" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>577.02734102703118</v>
       </c>
       <c r="I6" s="4">
-        <f>D6/G6</f>
+        <f t="shared" si="0"/>
         <v>0.19463087248322147</v>
       </c>
       <c r="J6" s="13">
-        <f t="shared" ref="J6:J23" si="4">AVERAGE(I3:I6)</f>
+        <f t="shared" ref="J6:J23" si="8">AVERAGE(I3:I6)</f>
         <v>0.17276118473632587</v>
       </c>
       <c r="K6" s="1">
-        <f>D6+K5</f>
+        <f t="shared" si="5"/>
         <v>167</v>
       </c>
       <c r="L6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>908</v>
       </c>
       <c r="M6" s="20"/>
@@ -5238,11 +5337,11 @@
       <c r="U6" s="20"/>
       <c r="V6" s="20"/>
       <c r="W6" t="str">
-        <f>IF(S6+Q6=D6,"EQUAL","DIFFER")</f>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="X6" t="str">
-        <f>IF(T6+R6=G6,"EQUAL","DIFFER")</f>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
       <c r="Z6" t="s">
@@ -5263,34 +5362,34 @@
         <v>15</v>
       </c>
       <c r="E7">
+        <f t="shared" si="7"/>
+        <v>44.25</v>
+      </c>
+      <c r="F7" s="24">
         <f t="shared" si="3"/>
-        <v>44.25</v>
-      </c>
-      <c r="F7" s="24">
-        <f t="shared" si="0"/>
         <v>58.090000774533344</v>
       </c>
       <c r="G7">
         <v>280</v>
       </c>
       <c r="H7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1084.3466811246224</v>
       </c>
       <c r="I7" s="4">
-        <f>D7/G7</f>
+        <f t="shared" si="0"/>
         <v>5.3571428571428568E-2</v>
       </c>
       <c r="J7" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.17916103488617602</v>
       </c>
       <c r="K7" s="1">
-        <f>D7+K6</f>
+        <f t="shared" si="5"/>
         <v>182</v>
       </c>
       <c r="L7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1188</v>
       </c>
       <c r="M7" s="20"/>
@@ -5312,11 +5411,11 @@
       <c r="U7" s="20"/>
       <c r="V7" s="20"/>
       <c r="W7" t="str">
-        <f>IF(S7+Q7=D7,"EQUAL","DIFFER")</f>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="X7" t="str">
-        <f>IF(T7+R7=G7,"EQUAL","DIFFER")</f>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -5334,34 +5433,34 @@
         <v>11</v>
       </c>
       <c r="E8">
+        <f t="shared" si="7"/>
+        <v>25.25</v>
+      </c>
+      <c r="F8" s="24">
         <f t="shared" si="3"/>
-        <v>25.25</v>
-      </c>
-      <c r="F8" s="24">
-        <f t="shared" si="0"/>
         <v>42.599333901324449</v>
       </c>
       <c r="G8">
         <v>84</v>
       </c>
       <c r="H8" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>325.30400433738674</v>
       </c>
       <c r="I8" s="4">
-        <f>D8/G8</f>
+        <f t="shared" si="0"/>
         <v>0.13095238095238096</v>
       </c>
       <c r="J8" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.13337927452860338</v>
       </c>
       <c r="K8" s="1">
-        <f>D8+K7</f>
+        <f t="shared" si="5"/>
         <v>193</v>
       </c>
       <c r="L8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1272</v>
       </c>
       <c r="M8" s="20"/>
@@ -5383,11 +5482,11 @@
       <c r="U8" s="20"/>
       <c r="V8" s="20"/>
       <c r="W8" t="str">
-        <f>IF(S8+Q8=D8,"EQUAL","DIFFER")</f>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="X8" t="str">
-        <f>IF(T8+R8=G8,"EQUAL","DIFFER")</f>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -5405,34 +5504,34 @@
         <v>54</v>
       </c>
       <c r="E9">
+        <f t="shared" si="7"/>
+        <v>27.25</v>
+      </c>
+      <c r="F9" s="24">
         <f t="shared" si="3"/>
-        <v>27.25</v>
-      </c>
-      <c r="F9" s="24">
-        <f t="shared" si="0"/>
         <v>209.12400278832004</v>
       </c>
       <c r="G9">
         <v>2230</v>
       </c>
       <c r="H9" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>8636.0467818139568</v>
       </c>
       <c r="I9" s="4">
-        <f>D9/G9</f>
+        <f t="shared" si="0"/>
         <v>2.4215246636771302E-2</v>
       </c>
       <c r="J9" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.10084248216095058</v>
       </c>
       <c r="K9" s="1">
-        <f>D9+K8</f>
+        <f t="shared" si="5"/>
         <v>247</v>
       </c>
       <c r="L9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3502</v>
       </c>
       <c r="M9" s="20"/>
@@ -5454,11 +5553,11 @@
       <c r="U9" s="20"/>
       <c r="V9" s="20"/>
       <c r="W9" t="str">
-        <f>IF(S9+Q9=D9,"EQUAL","DIFFER")</f>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="X9" t="str">
-        <f>IF(T9+R9=G9,"EQUAL","DIFFER")</f>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -5476,34 +5575,34 @@
         <v>19</v>
       </c>
       <c r="E10">
+        <f t="shared" si="7"/>
+        <v>24.75</v>
+      </c>
+      <c r="F10" s="24">
         <f t="shared" si="3"/>
-        <v>24.75</v>
-      </c>
-      <c r="F10" s="24">
-        <f t="shared" si="0"/>
         <v>73.580667647742231</v>
       </c>
       <c r="G10">
         <v>881</v>
       </c>
       <c r="H10" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3411.8193788242588</v>
       </c>
       <c r="I10" s="4">
-        <f>D10/G10</f>
+        <f t="shared" si="0"/>
         <v>2.1566401816118047E-2</v>
       </c>
       <c r="J10" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5.757636449417472E-2</v>
       </c>
       <c r="K10" s="1">
-        <f>D10+K9</f>
+        <f t="shared" si="5"/>
         <v>266</v>
       </c>
       <c r="L10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4383</v>
       </c>
       <c r="M10" s="20"/>
@@ -5525,11 +5624,11 @@
       <c r="U10" s="20"/>
       <c r="V10" s="20"/>
       <c r="W10" t="str">
-        <f>IF(S10+Q10=D10,"EQUAL","DIFFER")</f>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="X10" t="str">
-        <f>IF(T10+R10=G10,"EQUAL","DIFFER")</f>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -5547,34 +5646,34 @@
         <v>7</v>
       </c>
       <c r="E11">
+        <f t="shared" si="7"/>
+        <v>22.75</v>
+      </c>
+      <c r="F11" s="24">
         <f t="shared" si="3"/>
-        <v>22.75</v>
-      </c>
-      <c r="F11" s="24">
-        <f t="shared" si="0"/>
         <v>27.108667028115558</v>
       </c>
       <c r="G11">
         <v>783</v>
       </c>
       <c r="H11" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3032.2980404306404</v>
       </c>
       <c r="I11" s="4">
-        <f>D11/G11</f>
+        <f t="shared" si="0"/>
         <v>8.9399744572158362E-3</v>
       </c>
       <c r="J11" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4.6418500965621536E-2</v>
       </c>
       <c r="K11" s="1">
-        <f>D11+K10</f>
+        <f t="shared" si="5"/>
         <v>273</v>
       </c>
       <c r="L11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>5166</v>
       </c>
       <c r="M11" s="20"/>
@@ -5596,11 +5695,11 @@
       <c r="U11" s="20"/>
       <c r="V11" s="20"/>
       <c r="W11" t="str">
-        <f>IF(S11+Q11=D11,"EQUAL","DIFFER")</f>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="X11" t="str">
-        <f>IF(T11+R11=G11,"EQUAL","DIFFER")</f>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -5618,34 +5717,34 @@
         <v>7</v>
       </c>
       <c r="E12">
+        <f t="shared" si="7"/>
+        <v>21.75</v>
+      </c>
+      <c r="F12" s="24">
         <f t="shared" si="3"/>
-        <v>21.75</v>
-      </c>
-      <c r="F12" s="24">
-        <f t="shared" si="0"/>
         <v>27.108667028115558</v>
       </c>
       <c r="G12">
         <v>1037</v>
       </c>
       <c r="H12" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>4015.9553868794051</v>
       </c>
       <c r="I12" s="4">
-        <f>D12/G12</f>
+        <f t="shared" si="0"/>
         <v>6.7502410800385727E-3</v>
       </c>
       <c r="J12" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1.5367965997535938E-2</v>
       </c>
       <c r="K12" s="1">
-        <f>D12+K11</f>
+        <f t="shared" si="5"/>
         <v>280</v>
       </c>
       <c r="L12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>6203</v>
       </c>
       <c r="M12" s="20"/>
@@ -5667,11 +5766,11 @@
       <c r="U12" s="20"/>
       <c r="V12" s="20"/>
       <c r="W12" t="str">
-        <f>IF(S12+Q12=D12,"EQUAL","DIFFER")</f>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="X12" t="str">
-        <f>IF(T12+R12=G12,"EQUAL","DIFFER")</f>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -5689,34 +5788,34 @@
         <v>26</v>
       </c>
       <c r="E13">
+        <f t="shared" si="7"/>
+        <v>14.75</v>
+      </c>
+      <c r="F13" s="24">
         <f t="shared" si="3"/>
-        <v>14.75</v>
-      </c>
-      <c r="F13" s="24">
-        <f t="shared" si="0"/>
         <v>100.68933467585781</v>
       </c>
       <c r="G13">
         <v>1590</v>
       </c>
       <c r="H13" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>6157.5400821005342</v>
       </c>
       <c r="I13" s="4">
-        <f>D13/G13</f>
+        <f t="shared" si="0"/>
         <v>1.6352201257861635E-2</v>
       </c>
       <c r="J13" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1.3402204652808523E-2</v>
       </c>
       <c r="K13" s="1">
-        <f>D13+K12</f>
+        <f t="shared" si="5"/>
         <v>306</v>
       </c>
       <c r="L13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>7793</v>
       </c>
       <c r="M13" s="20"/>
@@ -5738,11 +5837,11 @@
       <c r="U13" s="20"/>
       <c r="V13" s="20"/>
       <c r="W13" t="str">
-        <f>IF(S13+Q13=D13,"EQUAL","DIFFER")</f>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="X13" t="str">
-        <f>IF(T13+R13=G13,"EQUAL","DIFFER")</f>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -5760,34 +5859,34 @@
         <v>173</v>
       </c>
       <c r="E14">
+        <f t="shared" si="7"/>
+        <v>53.25</v>
+      </c>
+      <c r="F14" s="24">
         <f t="shared" si="3"/>
-        <v>53.25</v>
-      </c>
-      <c r="F14" s="24">
-        <f t="shared" si="0"/>
         <v>669.97134226628464</v>
       </c>
       <c r="G14">
         <v>2188</v>
       </c>
       <c r="H14" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>8473.3947796452649</v>
       </c>
       <c r="I14" s="4">
-        <f>D14/G14</f>
+        <f t="shared" si="0"/>
         <v>7.906764168190128E-2</v>
       </c>
       <c r="J14" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2.7777514619254332E-2</v>
       </c>
       <c r="K14" s="1">
-        <f>D14+K13</f>
+        <f t="shared" si="5"/>
         <v>479</v>
       </c>
       <c r="L14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>9981</v>
       </c>
       <c r="M14">
@@ -5815,19 +5914,19 @@
         <v>1671</v>
       </c>
       <c r="U14" t="str">
-        <f>IF(M14+O14=D14,"EQUAL","DIFFER")</f>
+        <f t="shared" ref="U14:U23" si="9">IF(M14+O14=D14,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="V14" t="str">
-        <f>IF(N14+P14=G14,"EQUAL","DIFFER")</f>
+        <f t="shared" ref="V14:V23" si="10">IF(N14+P14=G14,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="W14" t="str">
-        <f>IF(S14+Q14=D14,"EQUAL","DIFFER")</f>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="X14" t="str">
-        <f>IF(T14+R14=G14,"EQUAL","DIFFER")</f>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -5845,34 +5944,34 @@
         <v>861</v>
       </c>
       <c r="E15">
+        <f t="shared" si="7"/>
+        <v>266.75</v>
+      </c>
+      <c r="F15" s="24">
         <f t="shared" si="3"/>
-        <v>266.75</v>
-      </c>
-      <c r="F15" s="24">
-        <f t="shared" si="0"/>
         <v>3334.3660444582138</v>
       </c>
       <c r="G15">
         <v>6986</v>
       </c>
       <c r="H15" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>27054.449694059331</v>
       </c>
       <c r="I15" s="4">
-        <f>D15/G15</f>
+        <f t="shared" si="0"/>
         <v>0.12324649298597194</v>
       </c>
       <c r="J15" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5.6354144251443361E-2</v>
       </c>
       <c r="K15" s="1">
-        <f>D15+K14</f>
+        <f t="shared" si="5"/>
         <v>1340</v>
       </c>
       <c r="L15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>16967</v>
       </c>
       <c r="M15">
@@ -5900,19 +5999,19 @@
         <v>6346</v>
       </c>
       <c r="U15" t="str">
-        <f>IF(M15+O15=D15,"EQUAL","DIFFER")</f>
+        <f t="shared" si="9"/>
         <v>EQUAL</v>
       </c>
       <c r="V15" t="str">
-        <f>IF(N15+P15=G15,"EQUAL","DIFFER")</f>
+        <f t="shared" si="10"/>
         <v>EQUAL</v>
       </c>
       <c r="W15" t="str">
-        <f>IF(S15+Q15=D15,"EQUAL","DIFFER")</f>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="X15" t="str">
-        <f>IF(T15+R15=G15,"EQUAL","DIFFER")</f>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -5930,34 +6029,34 @@
         <v>487</v>
       </c>
       <c r="E16">
+        <f t="shared" si="7"/>
+        <v>386.75</v>
+      </c>
+      <c r="F16" s="24">
         <f t="shared" si="3"/>
-        <v>386.75</v>
-      </c>
-      <c r="F16" s="24">
-        <f t="shared" si="0"/>
         <v>1885.9886918131826</v>
       </c>
       <c r="G16">
         <v>9254</v>
       </c>
       <c r="H16" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>35837.65781116877</v>
       </c>
       <c r="I16" s="4">
-        <f>D16/G16</f>
+        <f t="shared" si="0"/>
         <v>5.2625891506375623E-2</v>
       </c>
       <c r="J16" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>6.7823056858027628E-2</v>
       </c>
       <c r="K16" s="1">
-        <f>D16+K15</f>
+        <f t="shared" si="5"/>
         <v>1827</v>
       </c>
       <c r="L16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>26221</v>
       </c>
       <c r="M16">
@@ -5985,19 +6084,19 @@
         <v>8297</v>
       </c>
       <c r="U16" t="str">
-        <f>IF(M16+O16=D16,"EQUAL","DIFFER")</f>
+        <f t="shared" si="9"/>
         <v>EQUAL</v>
       </c>
       <c r="V16" t="str">
-        <f>IF(N16+P16=G16,"EQUAL","DIFFER")</f>
+        <f t="shared" si="10"/>
         <v>EQUAL</v>
       </c>
       <c r="W16" t="str">
-        <f>IF(S16+Q16=D16,"EQUAL","DIFFER")</f>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="X16" t="str">
-        <f>IF(T16+R16=G16,"EQUAL","DIFFER")</f>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -6015,34 +6114,34 @@
         <v>858</v>
       </c>
       <c r="E17">
+        <f t="shared" si="7"/>
+        <v>594.75</v>
+      </c>
+      <c r="F17" s="24">
         <f t="shared" si="3"/>
-        <v>594.75</v>
-      </c>
-      <c r="F17" s="24">
-        <f t="shared" si="0"/>
         <v>3322.7480443033073</v>
       </c>
       <c r="G17">
         <v>19442</v>
       </c>
       <c r="H17" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>75292.386337231816</v>
       </c>
       <c r="I17" s="4">
-        <f>D17/G17</f>
+        <f t="shared" si="0"/>
         <v>4.4131262215821421E-2</v>
       </c>
       <c r="J17" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>7.4767822097517575E-2</v>
       </c>
       <c r="K17" s="1">
-        <f>D17+K16</f>
+        <f t="shared" si="5"/>
         <v>2685</v>
       </c>
       <c r="L17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>45663</v>
       </c>
       <c r="M17">
@@ -6070,19 +6169,19 @@
         <v>18521</v>
       </c>
       <c r="U17" t="str">
-        <f>IF(M17+O17=D17,"EQUAL","DIFFER")</f>
+        <f t="shared" si="9"/>
         <v>EQUAL</v>
       </c>
       <c r="V17" t="str">
-        <f>IF(N17+P17=G17,"EQUAL","DIFFER")</f>
+        <f t="shared" si="10"/>
         <v>EQUAL</v>
       </c>
       <c r="W17" t="str">
-        <f>IF(S17+Q17=D17,"EQUAL","DIFFER")</f>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="X17" t="str">
-        <f>IF(T17+R17=G17,"EQUAL","DIFFER")</f>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -6100,34 +6199,34 @@
         <v>486</v>
       </c>
       <c r="E18">
+        <f t="shared" si="7"/>
+        <v>673</v>
+      </c>
+      <c r="F18" s="24">
         <f t="shared" si="3"/>
-        <v>673</v>
-      </c>
-      <c r="F18" s="24">
-        <f t="shared" si="0"/>
         <v>1882.1160250948803</v>
       </c>
       <c r="G18" s="9">
         <v>7698</v>
       </c>
       <c r="H18" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>29811.788397490513</v>
       </c>
       <c r="I18" s="4">
-        <f>D18/G18</f>
+        <f t="shared" si="0"/>
         <v>6.313328137178488E-2</v>
       </c>
       <c r="J18" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>7.0784232019988472E-2</v>
       </c>
       <c r="K18" s="1">
-        <f>D18+K17</f>
+        <f t="shared" si="5"/>
         <v>3171</v>
       </c>
       <c r="L18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>53361</v>
       </c>
       <c r="M18">
@@ -6155,19 +6254,19 @@
         <v>7265</v>
       </c>
       <c r="U18" t="str">
-        <f>IF(M18+O18=D18,"EQUAL","DIFFER")</f>
+        <f t="shared" si="9"/>
         <v>EQUAL</v>
       </c>
       <c r="V18" t="str">
-        <f>IF(N18+P18=G18,"EQUAL","DIFFER")</f>
+        <f t="shared" si="10"/>
         <v>EQUAL</v>
       </c>
       <c r="W18" t="str">
-        <f>IF(S18+Q18=D18,"EQUAL","DIFFER")</f>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="X18" t="str">
-        <f>IF(T18+R18=G18,"EQUAL","DIFFER")</f>
+        <f t="shared" si="2"/>
         <v>EQUAL</v>
       </c>
     </row>
@@ -6185,34 +6284,34 @@
         <v>588</v>
       </c>
       <c r="E19">
+        <f t="shared" si="7"/>
+        <v>604.75</v>
+      </c>
+      <c r="F19" s="24">
         <f t="shared" si="3"/>
-        <v>604.75</v>
-      </c>
-      <c r="F19" s="24">
-        <f t="shared" si="0"/>
         <v>2277.1280303617073</v>
       </c>
       <c r="G19" s="9">
         <v>8729</v>
       </c>
       <c r="H19" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>33804.507784060108</v>
       </c>
       <c r="I19" s="4">
-        <f>D19/G19</f>
+        <f t="shared" si="0"/>
         <v>6.7361668003207698E-2</v>
       </c>
       <c r="J19" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5.6813025774297407E-2</v>
       </c>
       <c r="K19" s="1">
-        <f>D19+K18</f>
+        <f t="shared" si="5"/>
         <v>3759</v>
       </c>
       <c r="L19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>62090</v>
       </c>
       <c r="M19">
@@ -6240,19 +6339,19 @@
         <v>8047</v>
       </c>
       <c r="U19" t="str">
-        <f>IF(M19+O19=D19,"EQUAL","DIFFER")</f>
+        <f t="shared" si="9"/>
         <v>EQUAL</v>
       </c>
       <c r="V19" t="str">
-        <f>IF(N19+P19=G19,"EQUAL","DIFFER")</f>
+        <f t="shared" si="10"/>
         <v>EQUAL</v>
       </c>
       <c r="W19" t="str">
-        <f>IF(S19+Q19=D19,"EQUAL","DIFFER")</f>
+        <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
       <c r="X19" t="str">
-        <f t="shared" ref="X19:X23" si="5">IF(T19+R19=G19,"EQUAL","DIFFER")</f>
+        <f t="shared" ref="X19:X23" si="11">IF(T19+R19=G19,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
     </row>
@@ -6270,51 +6369,75 @@
         <v>407</v>
       </c>
       <c r="E20">
+        <f t="shared" si="7"/>
+        <v>584.75</v>
+      </c>
+      <c r="F20" s="24">
         <f t="shared" si="3"/>
-        <v>584.75</v>
-      </c>
-      <c r="F20" s="24">
-        <f t="shared" si="0"/>
         <v>1576.1753543490047</v>
       </c>
       <c r="G20" s="9">
         <v>9224</v>
       </c>
       <c r="H20" s="9">
+        <f t="shared" si="4"/>
+        <v>35721.477809619704</v>
+      </c>
+      <c r="I20" s="4">
+        <f t="shared" si="0"/>
+        <v>4.4124024284475281E-2</v>
+      </c>
+      <c r="J20" s="13">
+        <f t="shared" si="8"/>
+        <v>5.4687558968822318E-2</v>
+      </c>
+      <c r="K20" s="1">
+        <f t="shared" si="5"/>
+        <v>4166</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="6"/>
+        <v>71314</v>
+      </c>
+      <c r="M20">
+        <v>35</v>
+      </c>
+      <c r="N20">
+        <v>96</v>
+      </c>
+      <c r="O20">
+        <v>372</v>
+      </c>
+      <c r="P20">
+        <v>9128</v>
+      </c>
+      <c r="Q20">
+        <v>6</v>
+      </c>
+      <c r="R20">
+        <v>1168</v>
+      </c>
+      <c r="S20">
+        <v>401</v>
+      </c>
+      <c r="T20">
+        <v>8056</v>
+      </c>
+      <c r="U20" t="str">
+        <f t="shared" si="9"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="V20" t="str">
+        <f t="shared" si="10"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="W20" t="str">
         <f t="shared" si="1"/>
-        <v>35721.477809619704</v>
-      </c>
-      <c r="I20" s="4">
-        <f>D20/G20</f>
-        <v>4.4124024284475281E-2</v>
-      </c>
-      <c r="J20" s="13">
-        <f t="shared" si="4"/>
-        <v>5.4687558968822318E-2</v>
-      </c>
-      <c r="K20" s="1">
-        <f>D20+K19</f>
-        <v>4166</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="2"/>
-        <v>71314</v>
-      </c>
-      <c r="U20" t="str">
-        <f>IF(M20+O20=D20,"EQUAL","DIFFER")</f>
-        <v>DIFFER</v>
-      </c>
-      <c r="V20" t="str">
-        <f>IF(N20+P20=G20,"EQUAL","DIFFER")</f>
-        <v>DIFFER</v>
-      </c>
-      <c r="W20" t="str">
-        <f>IF(S20+Q20=D20,"EQUAL","DIFFER")</f>
-        <v>DIFFER</v>
+        <v>EQUAL</v>
       </c>
       <c r="X20" t="str">
-        <f t="shared" si="5"/>
-        <v>DIFFER</v>
+        <f t="shared" si="11"/>
+        <v>EQUAL</v>
       </c>
     </row>
     <row r="21" spans="1:24">
@@ -6331,51 +6454,75 @@
         <v>249</v>
       </c>
       <c r="E21">
+        <f t="shared" si="7"/>
+        <v>432.5</v>
+      </c>
+      <c r="F21" s="24">
         <f t="shared" si="3"/>
-        <v>432.5</v>
-      </c>
-      <c r="F21" s="24">
-        <f t="shared" si="0"/>
         <v>964.29401285725351</v>
       </c>
       <c r="G21" s="9">
-        <v>9032</v>
+        <v>9033</v>
       </c>
       <c r="H21" s="9">
+        <f t="shared" si="4"/>
+        <v>34981.798466423978</v>
+      </c>
+      <c r="I21" s="4">
+        <f t="shared" si="0"/>
+        <v>2.7565592826303553E-2</v>
+      </c>
+      <c r="J21" s="13">
+        <f t="shared" si="8"/>
+        <v>5.0546141621442851E-2</v>
+      </c>
+      <c r="K21" s="1">
+        <f t="shared" si="5"/>
+        <v>4415</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="6"/>
+        <v>80347</v>
+      </c>
+      <c r="M21">
+        <v>29</v>
+      </c>
+      <c r="N21">
+        <v>96</v>
+      </c>
+      <c r="O21">
+        <v>220</v>
+      </c>
+      <c r="P21">
+        <v>8937</v>
+      </c>
+      <c r="Q21">
+        <v>14</v>
+      </c>
+      <c r="R21">
+        <v>1057</v>
+      </c>
+      <c r="S21">
+        <v>235</v>
+      </c>
+      <c r="T21">
+        <v>7976</v>
+      </c>
+      <c r="U21" t="str">
+        <f t="shared" si="9"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="V21" t="str">
+        <f t="shared" si="10"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="W21" t="str">
         <f t="shared" si="1"/>
-        <v>34977.925799705677</v>
-      </c>
-      <c r="I21" s="4">
-        <f>D21/G21</f>
-        <v>2.7568644818423384E-2</v>
-      </c>
-      <c r="J21" s="13">
-        <f t="shared" si="4"/>
-        <v>5.054690461947281E-2</v>
-      </c>
-      <c r="K21" s="1">
-        <f>D21+K20</f>
-        <v>4415</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="2"/>
-        <v>80346</v>
-      </c>
-      <c r="U21" t="str">
-        <f>IF(M21+O21=D21,"EQUAL","DIFFER")</f>
-        <v>DIFFER</v>
-      </c>
-      <c r="V21" t="str">
-        <f>IF(N21+P21=G21,"EQUAL","DIFFER")</f>
-        <v>DIFFER</v>
-      </c>
-      <c r="W21" t="str">
-        <f>IF(S21+Q21=D21,"EQUAL","DIFFER")</f>
-        <v>DIFFER</v>
+        <v>EQUAL</v>
       </c>
       <c r="X21" t="str">
-        <f t="shared" si="5"/>
-        <v>DIFFER</v>
+        <f t="shared" si="11"/>
+        <v>EQUAL</v>
       </c>
     </row>
     <row r="22" spans="1:24">
@@ -6389,54 +6536,78 @@
         <v>44128</v>
       </c>
       <c r="D22">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E22">
         <f>AVERAGE(D19:D22)</f>
-        <v>349.5</v>
+        <v>350</v>
       </c>
       <c r="F22" s="24">
-        <f t="shared" si="0"/>
-        <v>596.39067461854233</v>
+        <f t="shared" si="3"/>
+        <v>604.1360080551467</v>
       </c>
       <c r="G22" s="9">
-        <v>10423</v>
+        <v>10436</v>
       </c>
       <c r="H22" s="9">
+        <f t="shared" si="4"/>
+        <v>40415.149872201997</v>
+      </c>
+      <c r="I22" s="4">
+        <f t="shared" si="0"/>
+        <v>1.4948256036795707E-2</v>
+      </c>
+      <c r="J22" s="13">
+        <f t="shared" si="8"/>
+        <v>3.8499885287695559E-2</v>
+      </c>
+      <c r="K22" s="1">
+        <f t="shared" si="5"/>
+        <v>4571</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="6"/>
+        <v>90783</v>
+      </c>
+      <c r="M22">
+        <v>12</v>
+      </c>
+      <c r="N22">
+        <v>57</v>
+      </c>
+      <c r="O22">
+        <v>144</v>
+      </c>
+      <c r="P22">
+        <v>10379</v>
+      </c>
+      <c r="Q22">
+        <v>22</v>
+      </c>
+      <c r="R22">
+        <v>1488</v>
+      </c>
+      <c r="S22">
+        <v>134</v>
+      </c>
+      <c r="T22">
+        <v>8948</v>
+      </c>
+      <c r="U22" t="str">
+        <f t="shared" si="9"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="V22" t="str">
+        <f t="shared" si="10"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="W22" t="str">
         <f t="shared" si="1"/>
-        <v>40364.805204864067</v>
-      </c>
-      <c r="I22" s="4">
-        <f>D22/G22</f>
-        <v>1.4775016789791807E-2</v>
-      </c>
-      <c r="J22" s="13">
-        <f t="shared" si="4"/>
-        <v>3.8457338473974548E-2</v>
-      </c>
-      <c r="K22" s="1">
-        <f>D22+K21</f>
-        <v>4569</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="2"/>
-        <v>90769</v>
-      </c>
-      <c r="U22" t="str">
-        <f>IF(M22+O22=D22,"EQUAL","DIFFER")</f>
-        <v>DIFFER</v>
-      </c>
-      <c r="V22" t="str">
-        <f>IF(N22+P22=G22,"EQUAL","DIFFER")</f>
-        <v>DIFFER</v>
-      </c>
-      <c r="W22" t="str">
-        <f>IF(S22+Q22=D22,"EQUAL","DIFFER")</f>
-        <v>DIFFER</v>
+        <v>EQUAL</v>
       </c>
       <c r="X22" t="str">
-        <f t="shared" si="5"/>
-        <v>DIFFER</v>
+        <f t="shared" si="11"/>
+        <v>EQUAL</v>
       </c>
     </row>
     <row r="23" spans="1:24">
@@ -6447,57 +6618,81 @@
         <v>28</v>
       </c>
       <c r="C23" s="30">
-        <v>44133</v>
+        <v>44135</v>
       </c>
       <c r="D23">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="E23">
+        <f t="shared" si="7"/>
+        <v>225</v>
+      </c>
+      <c r="F23" s="24">
         <f t="shared" si="3"/>
-        <v>218.25</v>
-      </c>
-      <c r="F23" s="24">
-        <f t="shared" si="0"/>
-        <v>243.97800325304007</v>
+        <v>340.7946712105956</v>
       </c>
       <c r="G23" s="9">
-        <v>7384</v>
+        <v>9624</v>
       </c>
       <c r="H23" s="9">
+        <f t="shared" si="4"/>
+        <v>37270.544496940594</v>
+      </c>
+      <c r="I23" s="4">
+        <f t="shared" si="0"/>
+        <v>9.14380714879468E-3</v>
+      </c>
+      <c r="J23" s="13">
+        <f t="shared" si="8"/>
+        <v>2.3945420074092307E-2</v>
+      </c>
+      <c r="K23" s="1">
+        <f t="shared" si="5"/>
+        <v>4659</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="6"/>
+        <v>100407</v>
+      </c>
+      <c r="M23">
+        <v>4</v>
+      </c>
+      <c r="N23">
+        <v>51</v>
+      </c>
+      <c r="O23">
+        <v>84</v>
+      </c>
+      <c r="P23">
+        <v>9573</v>
+      </c>
+      <c r="Q23">
+        <v>6</v>
+      </c>
+      <c r="R23">
+        <v>1434</v>
+      </c>
+      <c r="S23">
+        <v>82</v>
+      </c>
+      <c r="T23">
+        <v>8190</v>
+      </c>
+      <c r="U23" t="str">
+        <f t="shared" si="9"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="V23" t="str">
+        <f t="shared" si="10"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="W23" t="str">
         <f t="shared" si="1"/>
-        <v>28595.771047943614</v>
-      </c>
-      <c r="I23" s="4">
-        <f>D23/G23</f>
-        <v>8.5319609967497295E-3</v>
-      </c>
-      <c r="J23" s="13">
-        <f t="shared" si="4"/>
-        <v>2.3749911722360049E-2</v>
-      </c>
-      <c r="K23" s="1">
-        <f>D23+K22</f>
-        <v>4632</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="2"/>
-        <v>98153</v>
-      </c>
-      <c r="U23" t="str">
-        <f>IF(M23+O23=D23,"EQUAL","DIFFER")</f>
-        <v>DIFFER</v>
-      </c>
-      <c r="V23" t="str">
-        <f>IF(N23+P23=G23,"EQUAL","DIFFER")</f>
-        <v>DIFFER</v>
-      </c>
-      <c r="W23" t="str">
-        <f>IF(S23+Q23=D23,"EQUAL","DIFFER")</f>
-        <v>DIFFER</v>
+        <v>EQUAL</v>
       </c>
       <c r="X23" t="str">
-        <f t="shared" si="5"/>
-        <v>DIFFER</v>
+        <f t="shared" si="11"/>
+        <v>EQUAL</v>
       </c>
     </row>
     <row r="24" spans="1:24">
@@ -6538,10 +6733,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE67BA8-2D94-544F-9655-C971E88AFA0C}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView zoomScale="124" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6606,7 +6801,7 @@
         <v>289</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D11" si="0">B5+C5</f>
+        <f t="shared" ref="D5:D13" si="0">B5+C5</f>
         <v>532</v>
       </c>
     </row>
@@ -6698,6 +6893,21 @@
       <c r="D11">
         <f t="shared" si="0"/>
         <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2">
+        <v>44137</v>
+      </c>
+      <c r="B12" s="9">
+        <v>42</v>
+      </c>
+      <c r="C12">
+        <v>40</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated dataset to include EOW Nov 7
</commit_message>
<xml_diff>
--- a/clemsonDashboard.xlsx
+++ b/clemsonDashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidferrara/Documents/Clemson/The Tiger/COVID-19/Data/ttn-clemson-covid-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325C45C1-20E2-CF4C-8F21-715AAFC96190}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5E2068-DB46-6E4D-9692-DB80932DA2D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="460" windowWidth="28040" windowHeight="16260" xr2:uid="{663FE1B6-0B7E-E04A-924C-6AB15F4F5852}"/>
+    <workbookView xWindow="340" yWindow="460" windowWidth="28040" windowHeight="16260" activeTab="1" xr2:uid="{663FE1B6-0B7E-E04A-924C-6AB15F4F5852}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Data" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -800,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2018E299-360B-F244-BDDD-9B449D0B7C0F}">
   <dimension ref="A1:X71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4895,8 +4895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D56922A-034D-7E4D-80AB-A29316427207}">
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5025,7 +5025,7 @@
         <v>158.77933545039113</v>
       </c>
       <c r="I2" s="4">
-        <f t="shared" ref="I2:I23" si="0">D2/G2</f>
+        <f t="shared" ref="I2:I24" si="0">D2/G2</f>
         <v>2.4390243902439025E-2</v>
       </c>
       <c r="J2" s="23"/>
@@ -5082,14 +5082,14 @@
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="24">
-        <f t="shared" ref="F3:F23" si="3">(D3/25822)*100000</f>
+        <f t="shared" ref="F3:F24" si="3">(D3/25822)*100000</f>
         <v>15.490666873208893</v>
       </c>
       <c r="G3">
         <v>143</v>
       </c>
       <c r="H3" s="9">
-        <f t="shared" ref="H3:H23" si="4">(G3/25822)*100000</f>
+        <f t="shared" ref="H3:H24" si="4">(G3/25822)*100000</f>
         <v>553.79134071721785</v>
       </c>
       <c r="I3" s="4">
@@ -5098,7 +5098,7 @@
       </c>
       <c r="J3" s="23"/>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K23" si="5">D3+K2</f>
+        <f t="shared" ref="K3:K24" si="5">D3+K2</f>
         <v>5</v>
       </c>
       <c r="L3">
@@ -5170,7 +5170,7 @@
         <v>92</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L23" si="6">G4+L3</f>
+        <f t="shared" ref="L4:L24" si="6">G4+L3</f>
         <v>461</v>
       </c>
       <c r="M4" s="20"/>
@@ -5288,7 +5288,7 @@
         <v>29</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E23" si="7">AVERAGE(D3:D6)</f>
+        <f t="shared" ref="E6:E24" si="7">AVERAGE(D3:D6)</f>
         <v>41.5</v>
       </c>
       <c r="F6" s="24">
@@ -5307,7 +5307,7 @@
         <v>0.19463087248322147</v>
       </c>
       <c r="J6" s="13">
-        <f t="shared" ref="J6:J23" si="8">AVERAGE(I3:I6)</f>
+        <f t="shared" ref="J6:J24" si="8">AVERAGE(I3:I6)</f>
         <v>0.17276118473632587</v>
       </c>
       <c r="K6" s="1">
@@ -6356,13 +6356,13 @@
       </c>
     </row>
     <row r="20" spans="1:24">
-      <c r="A20" s="26">
+      <c r="A20" s="5">
         <v>44108</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="29">
+      <c r="C20" s="28">
         <v>44114</v>
       </c>
       <c r="D20">
@@ -6696,9 +6696,89 @@
       </c>
     </row>
     <row r="24" spans="1:24">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+      <c r="A24" s="26">
+        <v>44136</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="26">
+        <v>44142</v>
+      </c>
+      <c r="D24">
+        <v>77</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="7"/>
+        <v>142.5</v>
+      </c>
+      <c r="F24" s="24">
+        <f t="shared" si="3"/>
+        <v>298.19533730927117</v>
+      </c>
+      <c r="G24" s="9">
+        <v>4938</v>
+      </c>
+      <c r="H24" s="9">
+        <f t="shared" si="4"/>
+        <v>19123.228254976377</v>
+      </c>
+      <c r="I24" s="4">
+        <f t="shared" si="0"/>
+        <v>1.5593357634669907E-2</v>
+      </c>
+      <c r="J24" s="13">
+        <f t="shared" si="8"/>
+        <v>1.6812753411640961E-2</v>
+      </c>
+      <c r="K24" s="1">
+        <f t="shared" si="5"/>
+        <v>4736</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="6"/>
+        <v>105345</v>
+      </c>
+      <c r="M24">
+        <v>2</v>
+      </c>
+      <c r="N24">
+        <v>24</v>
+      </c>
+      <c r="O24">
+        <v>75</v>
+      </c>
+      <c r="P24">
+        <v>4914</v>
+      </c>
+      <c r="Q24">
+        <v>6</v>
+      </c>
+      <c r="R24">
+        <v>881</v>
+      </c>
+      <c r="S24">
+        <v>71</v>
+      </c>
+      <c r="T24">
+        <v>4057</v>
+      </c>
+      <c r="U24" t="str">
+        <f t="shared" ref="U24" si="12">IF(M24+O24=D24,"EQUAL","DIFFER")</f>
+        <v>EQUAL</v>
+      </c>
+      <c r="V24" t="str">
+        <f t="shared" ref="V24" si="13">IF(N24+P24=G24,"EQUAL","DIFFER")</f>
+        <v>EQUAL</v>
+      </c>
+      <c r="W24" t="str">
+        <f t="shared" ref="W24" si="14">IF(S24+Q24=D24,"EQUAL","DIFFER")</f>
+        <v>EQUAL</v>
+      </c>
+      <c r="X24" t="str">
+        <f t="shared" ref="X24" si="15">IF(T24+R24=G24,"EQUAL","DIFFER")</f>
+        <v>EQUAL</v>
+      </c>
     </row>
     <row r="25" spans="1:24">
       <c r="A25" s="2"/>
@@ -6725,7 +6805,7 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="E5:E23" formulaRange="1"/>
+    <ignoredError sqref="E5:E24" formulaRange="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -6733,10 +6813,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE67BA8-2D94-544F-9655-C971E88AFA0C}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView zoomScale="124" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6910,6 +6990,21 @@
         <v>82</v>
       </c>
     </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2">
+        <v>44140</v>
+      </c>
+      <c r="B13" s="9">
+        <v>38</v>
+      </c>
+      <c r="C13">
+        <v>36</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add captions to all graphs
</commit_message>
<xml_diff>
--- a/clemsonDashboard.xlsx
+++ b/clemsonDashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidferrara/Documents/Clemson/The Tiger/COVID-19/Data/ttn-clemson-covid-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5E2068-DB46-6E4D-9692-DB80932DA2D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA86DA6-1FFD-2842-9DB0-D4212C014C82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="460" windowWidth="28040" windowHeight="16260" activeTab="1" xr2:uid="{663FE1B6-0B7E-E04A-924C-6AB15F4F5852}"/>
   </bookViews>
@@ -4896,7 +4896,7 @@
   <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Attempt to make a table in Tableau with expanded dimension
</commit_message>
<xml_diff>
--- a/clemsonDashboard.xlsx
+++ b/clemsonDashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidferrara/Documents/Clemson/The Tiger/COVID-19/Data/ttn-clemson-covid-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA86DA6-1FFD-2842-9DB0-D4212C014C82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DAF02B-CBC9-5245-B9A8-B0A36BE0FFD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="460" windowWidth="28040" windowHeight="16260" activeTab="1" xr2:uid="{663FE1B6-0B7E-E04A-924C-6AB15F4F5852}"/>
   </bookViews>
@@ -40,7 +40,7 @@
     <author>David Ferrara</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{EC62B871-9C18-4743-82CE-15ABB4BFA0D9}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{EC62B871-9C18-4743-82CE-15ABB4BFA0D9}">
       <text>
         <r>
           <rPr>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -257,6 +257,12 @@
   <si>
     <t>Tests per Capita (100k)</t>
   </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>CU</t>
+  </si>
 </sst>
 </file>
 
@@ -374,7 +380,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -420,6 +426,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -4893,10 +4902,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D56922A-034D-7E4D-80AB-A29316427207}">
-  <dimension ref="A1:Z25"/>
+  <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D2" sqref="D2:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4904,28 +4913,29 @@
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="3.1640625" customWidth="1"/>
     <col min="3" max="3" width="8.83203125" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.5" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1640625" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.6640625" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.83203125" customWidth="1"/>
-    <col min="13" max="13" width="27" customWidth="1"/>
-    <col min="14" max="14" width="22.33203125" customWidth="1"/>
-    <col min="15" max="16" width="23.6640625" customWidth="1"/>
-    <col min="17" max="17" width="16" customWidth="1"/>
-    <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="19" max="19" width="14.6640625" customWidth="1"/>
-    <col min="20" max="20" width="12.1640625" customWidth="1"/>
-    <col min="21" max="21" width="17.1640625" customWidth="1"/>
-    <col min="22" max="22" width="14.6640625" customWidth="1"/>
-    <col min="23" max="23" width="16.6640625" customWidth="1"/>
-    <col min="24" max="24" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="21.5" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.1640625" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.6640625" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="19.83203125" customWidth="1"/>
+    <col min="14" max="14" width="27" customWidth="1"/>
+    <col min="15" max="15" width="22.33203125" customWidth="1"/>
+    <col min="16" max="17" width="23.6640625" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
+    <col min="19" max="19" width="14" customWidth="1"/>
+    <col min="20" max="20" width="14.6640625" customWidth="1"/>
+    <col min="21" max="21" width="12.1640625" customWidth="1"/>
+    <col min="22" max="22" width="17.1640625" customWidth="1"/>
+    <col min="23" max="23" width="14.6640625" customWidth="1"/>
+    <col min="24" max="24" width="16.6640625" customWidth="1"/>
+    <col min="25" max="25" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="17" customHeight="1">
+    <row r="1" spans="1:27" ht="17" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -4936,70 +4946,73 @@
         <v>26</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="17" customHeight="1">
+    <row r="2" spans="1:27" ht="17" customHeight="1">
       <c r="A2" s="25">
         <v>43987</v>
       </c>
@@ -5009,65 +5022,68 @@
       <c r="C2" s="27">
         <v>43988</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="9">
         <v>1</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="24">
-        <f>(D2/25822)*100000</f>
+      <c r="F2" s="20"/>
+      <c r="G2" s="24">
+        <f>(E2/25822)*100000</f>
         <v>3.8726667183022232</v>
       </c>
-      <c r="G2" s="9">
+      <c r="H2" s="9">
         <v>41</v>
       </c>
-      <c r="H2" s="9">
-        <f>(G2/25822)*100000</f>
+      <c r="I2" s="9">
+        <f>(H2/25822)*100000</f>
         <v>158.77933545039113</v>
       </c>
-      <c r="I2" s="4">
-        <f t="shared" ref="I2:I24" si="0">D2/G2</f>
+      <c r="J2" s="4">
+        <f t="shared" ref="J2:J24" si="0">E2/H2</f>
         <v>2.4390243902439025E-2</v>
       </c>
-      <c r="J2" s="23"/>
-      <c r="K2" s="14">
-        <f>D2</f>
+      <c r="K2" s="23"/>
+      <c r="L2" s="14">
+        <f>E2</f>
         <v>1</v>
       </c>
-      <c r="L2" s="9">
-        <f>G2</f>
+      <c r="M2" s="9">
+        <f>H2</f>
         <v>41</v>
       </c>
-      <c r="M2" s="21"/>
       <c r="N2" s="21"/>
       <c r="O2" s="21"/>
       <c r="P2" s="21"/>
-      <c r="Q2">
+      <c r="Q2" s="21"/>
+      <c r="R2">
         <v>0</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>32</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>1</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>9</v>
       </c>
-      <c r="U2" s="20"/>
       <c r="V2" s="20"/>
-      <c r="W2" t="str">
-        <f t="shared" ref="W2:W23" si="1">IF(S2+Q2=D2,"EQUAL","DIFFER")</f>
-        <v>EQUAL</v>
-      </c>
+      <c r="W2" s="20"/>
       <c r="X2" t="str">
-        <f t="shared" ref="X2:X18" si="2">IF(T2+R2=G2,"EQUAL","DIFFER")</f>
-        <v>EQUAL</v>
-      </c>
-      <c r="Z2" t="s">
+        <f t="shared" ref="X2:X23" si="1">IF(T2+R2=E2,"EQUAL","DIFFER")</f>
+        <v>EQUAL</v>
+      </c>
+      <c r="Y2" t="str">
+        <f t="shared" ref="Y2:Y18" si="2">IF(U2+S2=H2,"EQUAL","DIFFER")</f>
+        <v>EQUAL</v>
+      </c>
+      <c r="AA2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:27">
       <c r="A3" s="5">
         <v>43989</v>
       </c>
@@ -5077,65 +5093,68 @@
       <c r="C3" s="28">
         <v>43995</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3">
         <v>4</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="24">
-        <f t="shared" ref="F3:F24" si="3">(D3/25822)*100000</f>
+      <c r="F3" s="20"/>
+      <c r="G3" s="24">
+        <f t="shared" ref="G3:G24" si="3">(E3/25822)*100000</f>
         <v>15.490666873208893</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>143</v>
       </c>
-      <c r="H3" s="9">
-        <f t="shared" ref="H3:H24" si="4">(G3/25822)*100000</f>
+      <c r="I3" s="9">
+        <f t="shared" ref="I3:I24" si="4">(H3/25822)*100000</f>
         <v>553.79134071721785</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="4">
         <f t="shared" si="0"/>
         <v>2.7972027972027972E-2</v>
       </c>
-      <c r="J3" s="23"/>
-      <c r="K3" s="1">
-        <f t="shared" ref="K3:K24" si="5">D3+K2</f>
+      <c r="K3" s="23"/>
+      <c r="L3" s="1">
+        <f t="shared" ref="L3:L24" si="5">E3+L2</f>
         <v>5</v>
       </c>
-      <c r="L3">
-        <f>G3+L2</f>
+      <c r="M3">
+        <f>H3+M2</f>
         <v>184</v>
       </c>
-      <c r="M3" s="20"/>
       <c r="N3" s="20"/>
       <c r="O3" s="20"/>
       <c r="P3" s="20"/>
-      <c r="Q3" s="9">
+      <c r="Q3" s="20"/>
+      <c r="R3" s="9">
         <v>0</v>
       </c>
-      <c r="R3" s="9">
+      <c r="S3" s="9">
         <v>2</v>
       </c>
-      <c r="S3" s="9">
+      <c r="T3" s="9">
         <v>4</v>
       </c>
-      <c r="T3" s="9">
+      <c r="U3" s="9">
         <v>141</v>
       </c>
-      <c r="U3" s="20"/>
       <c r="V3" s="20"/>
-      <c r="W3" t="str">
+      <c r="W3" s="20"/>
+      <c r="X3" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X3" t="str">
-        <f t="shared" si="2"/>
-        <v>EQUAL</v>
-      </c>
-      <c r="Z3" t="s">
+      <c r="Y3" t="str">
+        <f t="shared" si="2"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="AA3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:27">
       <c r="A4" s="5">
         <v>43996</v>
       </c>
@@ -5145,62 +5164,65 @@
       <c r="C4" s="28">
         <v>44002</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4">
         <v>87</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="24">
+      <c r="F4" s="20"/>
+      <c r="G4" s="24">
         <f t="shared" si="3"/>
         <v>336.92200449229341</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>277</v>
       </c>
-      <c r="H4" s="9">
+      <c r="I4" s="9">
         <f t="shared" si="4"/>
         <v>1072.7286809697157</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="4">
         <f t="shared" si="0"/>
         <v>0.3140794223826715</v>
       </c>
-      <c r="J4" s="23"/>
-      <c r="K4" s="1">
+      <c r="K4" s="23"/>
+      <c r="L4" s="1">
         <f t="shared" si="5"/>
         <v>92</v>
       </c>
-      <c r="L4">
-        <f t="shared" ref="L4:L24" si="6">G4+L3</f>
+      <c r="M4">
+        <f t="shared" ref="M4:M24" si="6">H4+M3</f>
         <v>461</v>
       </c>
-      <c r="M4" s="20"/>
       <c r="N4" s="20"/>
       <c r="O4" s="20"/>
       <c r="P4" s="20"/>
-      <c r="Q4" s="9">
+      <c r="Q4" s="20"/>
+      <c r="R4" s="9">
         <v>2</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>56</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>85</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>221</v>
       </c>
-      <c r="U4" s="20"/>
       <c r="V4" s="20"/>
-      <c r="W4" t="str">
+      <c r="W4" s="20"/>
+      <c r="X4" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X4" t="str">
-        <f t="shared" si="2"/>
-        <v>EQUAL</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26">
+      <c r="Y4" t="str">
+        <f t="shared" si="2"/>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27">
       <c r="A5" s="5">
         <v>44003</v>
       </c>
@@ -5210,71 +5232,74 @@
       <c r="C5" s="28">
         <v>44009</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5">
         <v>46</v>
       </c>
-      <c r="E5">
-        <f>AVERAGE(D2:D5)</f>
+      <c r="F5">
+        <f>AVERAGE(E2:E5)</f>
         <v>34.5</v>
       </c>
-      <c r="F5" s="24">
+      <c r="G5" s="24">
         <f t="shared" si="3"/>
         <v>178.14266904190225</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>298</v>
       </c>
-      <c r="H5" s="9">
+      <c r="I5" s="9">
         <f t="shared" si="4"/>
         <v>1154.0546820540624</v>
       </c>
-      <c r="I5" s="4">
+      <c r="J5" s="4">
         <f t="shared" si="0"/>
         <v>0.15436241610738255</v>
       </c>
-      <c r="J5" s="13">
-        <f>AVERAGE(I2:I5)</f>
+      <c r="K5" s="13">
+        <f>AVERAGE(J2:J5)</f>
         <v>0.13020102759113028</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <f t="shared" si="5"/>
         <v>138</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <f t="shared" si="6"/>
         <v>759</v>
       </c>
-      <c r="M5" s="20"/>
       <c r="N5" s="20"/>
       <c r="O5" s="20"/>
       <c r="P5" s="20"/>
-      <c r="Q5">
+      <c r="Q5" s="20"/>
+      <c r="R5">
         <v>1</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>78</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>45</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>220</v>
       </c>
-      <c r="U5" s="20"/>
       <c r="V5" s="20"/>
-      <c r="W5" t="str">
+      <c r="W5" s="20"/>
+      <c r="X5" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X5" t="str">
-        <f t="shared" si="2"/>
-        <v>EQUAL</v>
-      </c>
-      <c r="Z5" t="s">
+      <c r="Y5" t="str">
+        <f t="shared" si="2"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="AA5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:27">
       <c r="A6" s="5">
         <v>44010</v>
       </c>
@@ -5284,71 +5309,74 @@
       <c r="C6" s="28">
         <v>44016</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6">
         <v>29</v>
       </c>
-      <c r="E6">
-        <f t="shared" ref="E6:E24" si="7">AVERAGE(D3:D6)</f>
+      <c r="F6">
+        <f t="shared" ref="F6:F24" si="7">AVERAGE(E3:E6)</f>
         <v>41.5</v>
       </c>
-      <c r="F6" s="24">
+      <c r="G6" s="24">
         <f t="shared" si="3"/>
         <v>112.30733483076447</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>149</v>
       </c>
-      <c r="H6" s="9">
+      <c r="I6" s="9">
         <f t="shared" si="4"/>
         <v>577.02734102703118</v>
       </c>
-      <c r="I6" s="4">
+      <c r="J6" s="4">
         <f t="shared" si="0"/>
         <v>0.19463087248322147</v>
       </c>
-      <c r="J6" s="13">
-        <f t="shared" ref="J6:J24" si="8">AVERAGE(I3:I6)</f>
+      <c r="K6" s="13">
+        <f t="shared" ref="K6:K24" si="8">AVERAGE(J3:J6)</f>
         <v>0.17276118473632587</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <f t="shared" si="5"/>
         <v>167</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <f t="shared" si="6"/>
         <v>908</v>
       </c>
-      <c r="M6" s="20"/>
       <c r="N6" s="20"/>
       <c r="O6" s="20"/>
       <c r="P6" s="20"/>
-      <c r="Q6">
+      <c r="Q6" s="20"/>
+      <c r="R6">
         <v>4</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>17</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>25</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>132</v>
       </c>
-      <c r="U6" s="20"/>
       <c r="V6" s="20"/>
-      <c r="W6" t="str">
+      <c r="W6" s="20"/>
+      <c r="X6" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X6" t="str">
-        <f t="shared" si="2"/>
-        <v>EQUAL</v>
-      </c>
-      <c r="Z6" t="s">
+      <c r="Y6" t="str">
+        <f t="shared" si="2"/>
+        <v>EQUAL</v>
+      </c>
+      <c r="AA6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:27">
       <c r="A7" s="5">
         <v>44017</v>
       </c>
@@ -5358,68 +5386,71 @@
       <c r="C7" s="28">
         <v>44023</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7">
         <v>15</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <f t="shared" si="7"/>
         <v>44.25</v>
       </c>
-      <c r="F7" s="24">
+      <c r="G7" s="24">
         <f t="shared" si="3"/>
         <v>58.090000774533344</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>280</v>
       </c>
-      <c r="H7" s="9">
+      <c r="I7" s="9">
         <f t="shared" si="4"/>
         <v>1084.3466811246224</v>
       </c>
-      <c r="I7" s="4">
+      <c r="J7" s="4">
         <f t="shared" si="0"/>
         <v>5.3571428571428568E-2</v>
       </c>
-      <c r="J7" s="13">
+      <c r="K7" s="13">
         <f t="shared" si="8"/>
         <v>0.17916103488617602</v>
       </c>
-      <c r="K7" s="1">
+      <c r="L7" s="1">
         <f t="shared" si="5"/>
         <v>182</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <f t="shared" si="6"/>
         <v>1188</v>
       </c>
-      <c r="M7" s="20"/>
       <c r="N7" s="20"/>
       <c r="O7" s="20"/>
       <c r="P7" s="20"/>
-      <c r="Q7">
+      <c r="Q7" s="20"/>
+      <c r="R7">
         <v>3</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>87</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>12</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>193</v>
       </c>
-      <c r="U7" s="20"/>
       <c r="V7" s="20"/>
-      <c r="W7" t="str">
+      <c r="W7" s="20"/>
+      <c r="X7" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X7" t="str">
-        <f t="shared" si="2"/>
-        <v>EQUAL</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26">
+      <c r="Y7" t="str">
+        <f t="shared" si="2"/>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27">
       <c r="A8" s="5">
         <v>44024</v>
       </c>
@@ -5429,68 +5460,71 @@
       <c r="C8" s="28">
         <v>44030</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8">
         <v>11</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <f t="shared" si="7"/>
         <v>25.25</v>
       </c>
-      <c r="F8" s="24">
+      <c r="G8" s="24">
         <f t="shared" si="3"/>
         <v>42.599333901324449</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>84</v>
       </c>
-      <c r="H8" s="9">
+      <c r="I8" s="9">
         <f t="shared" si="4"/>
         <v>325.30400433738674</v>
       </c>
-      <c r="I8" s="4">
+      <c r="J8" s="4">
         <f t="shared" si="0"/>
         <v>0.13095238095238096</v>
       </c>
-      <c r="J8" s="13">
+      <c r="K8" s="13">
         <f t="shared" si="8"/>
         <v>0.13337927452860338</v>
       </c>
-      <c r="K8" s="1">
+      <c r="L8" s="1">
         <f t="shared" si="5"/>
         <v>193</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <f t="shared" si="6"/>
         <v>1272</v>
       </c>
-      <c r="M8" s="20"/>
       <c r="N8" s="20"/>
       <c r="O8" s="20"/>
       <c r="P8" s="20"/>
-      <c r="Q8">
+      <c r="Q8" s="20"/>
+      <c r="R8">
         <v>2</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>29</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>9</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>55</v>
       </c>
-      <c r="U8" s="20"/>
       <c r="V8" s="20"/>
-      <c r="W8" t="str">
+      <c r="W8" s="20"/>
+      <c r="X8" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X8" t="str">
-        <f t="shared" si="2"/>
-        <v>EQUAL</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26">
+      <c r="Y8" t="str">
+        <f t="shared" si="2"/>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27">
       <c r="A9" s="5">
         <v>44031</v>
       </c>
@@ -5500,68 +5534,71 @@
       <c r="C9" s="28">
         <v>44037</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9">
         <v>54</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <f t="shared" si="7"/>
         <v>27.25</v>
       </c>
-      <c r="F9" s="24">
+      <c r="G9" s="24">
         <f t="shared" si="3"/>
         <v>209.12400278832004</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>2230</v>
       </c>
-      <c r="H9" s="9">
+      <c r="I9" s="9">
         <f t="shared" si="4"/>
         <v>8636.0467818139568</v>
       </c>
-      <c r="I9" s="4">
+      <c r="J9" s="4">
         <f t="shared" si="0"/>
         <v>2.4215246636771302E-2</v>
       </c>
-      <c r="J9" s="13">
+      <c r="K9" s="13">
         <f t="shared" si="8"/>
         <v>0.10084248216095058</v>
       </c>
-      <c r="K9" s="1">
+      <c r="L9" s="1">
         <f t="shared" si="5"/>
         <v>247</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <f t="shared" si="6"/>
         <v>3502</v>
       </c>
-      <c r="M9" s="20"/>
       <c r="N9" s="20"/>
       <c r="O9" s="20"/>
       <c r="P9" s="20"/>
-      <c r="Q9">
+      <c r="Q9" s="20"/>
+      <c r="R9">
         <v>34</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>1649</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>20</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>581</v>
       </c>
-      <c r="U9" s="20"/>
       <c r="V9" s="20"/>
-      <c r="W9" t="str">
+      <c r="W9" s="20"/>
+      <c r="X9" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X9" t="str">
-        <f t="shared" si="2"/>
-        <v>EQUAL</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26">
+      <c r="Y9" t="str">
+        <f t="shared" si="2"/>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27">
       <c r="A10" s="5">
         <v>44038</v>
       </c>
@@ -5571,68 +5608,71 @@
       <c r="C10" s="28">
         <v>44044</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10">
         <v>19</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <f t="shared" si="7"/>
         <v>24.75</v>
       </c>
-      <c r="F10" s="24">
+      <c r="G10" s="24">
         <f t="shared" si="3"/>
         <v>73.580667647742231</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>881</v>
       </c>
-      <c r="H10" s="9">
+      <c r="I10" s="9">
         <f t="shared" si="4"/>
         <v>3411.8193788242588</v>
       </c>
-      <c r="I10" s="4">
+      <c r="J10" s="4">
         <f t="shared" si="0"/>
         <v>2.1566401816118047E-2</v>
       </c>
-      <c r="J10" s="13">
+      <c r="K10" s="13">
         <f t="shared" si="8"/>
         <v>5.757636449417472E-2</v>
       </c>
-      <c r="K10" s="1">
+      <c r="L10" s="1">
         <f t="shared" si="5"/>
         <v>266</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <f t="shared" si="6"/>
         <v>4383</v>
       </c>
-      <c r="M10" s="20"/>
       <c r="N10" s="20"/>
       <c r="O10" s="20"/>
       <c r="P10" s="20"/>
-      <c r="Q10">
+      <c r="Q10" s="20"/>
+      <c r="R10">
         <v>9</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>590</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>10</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>291</v>
       </c>
-      <c r="U10" s="20"/>
       <c r="V10" s="20"/>
-      <c r="W10" t="str">
+      <c r="W10" s="20"/>
+      <c r="X10" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X10" t="str">
-        <f t="shared" si="2"/>
-        <v>EQUAL</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26">
+      <c r="Y10" t="str">
+        <f t="shared" si="2"/>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27">
       <c r="A11" s="5">
         <v>44045</v>
       </c>
@@ -5642,68 +5682,71 @@
       <c r="C11" s="28">
         <v>44051</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11">
         <v>7</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <f t="shared" si="7"/>
         <v>22.75</v>
       </c>
-      <c r="F11" s="24">
+      <c r="G11" s="24">
         <f t="shared" si="3"/>
         <v>27.108667028115558</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>783</v>
       </c>
-      <c r="H11" s="9">
+      <c r="I11" s="9">
         <f t="shared" si="4"/>
         <v>3032.2980404306404</v>
       </c>
-      <c r="I11" s="4">
+      <c r="J11" s="4">
         <f t="shared" si="0"/>
         <v>8.9399744572158362E-3</v>
       </c>
-      <c r="J11" s="13">
+      <c r="K11" s="13">
         <f t="shared" si="8"/>
         <v>4.6418500965621536E-2</v>
       </c>
-      <c r="K11" s="1">
+      <c r="L11" s="1">
         <f t="shared" si="5"/>
         <v>273</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <f t="shared" si="6"/>
         <v>5166</v>
       </c>
-      <c r="M11" s="20"/>
       <c r="N11" s="20"/>
       <c r="O11" s="20"/>
       <c r="P11" s="20"/>
-      <c r="Q11">
+      <c r="Q11" s="20"/>
+      <c r="R11">
         <v>2</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>365</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>5</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>418</v>
       </c>
-      <c r="U11" s="20"/>
       <c r="V11" s="20"/>
-      <c r="W11" t="str">
+      <c r="W11" s="20"/>
+      <c r="X11" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X11" t="str">
-        <f t="shared" si="2"/>
-        <v>EQUAL</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26">
+      <c r="Y11" t="str">
+        <f t="shared" si="2"/>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27">
       <c r="A12" s="5">
         <v>44052</v>
       </c>
@@ -5713,68 +5756,71 @@
       <c r="C12" s="28">
         <v>44058</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12">
         <v>7</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <f t="shared" si="7"/>
         <v>21.75</v>
       </c>
-      <c r="F12" s="24">
+      <c r="G12" s="24">
         <f t="shared" si="3"/>
         <v>27.108667028115558</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>1037</v>
       </c>
-      <c r="H12" s="9">
+      <c r="I12" s="9">
         <f t="shared" si="4"/>
         <v>4015.9553868794051</v>
       </c>
-      <c r="I12" s="4">
+      <c r="J12" s="4">
         <f t="shared" si="0"/>
         <v>6.7502410800385727E-3</v>
       </c>
-      <c r="J12" s="13">
+      <c r="K12" s="13">
         <f t="shared" si="8"/>
         <v>1.5367965997535938E-2</v>
       </c>
-      <c r="K12" s="1">
+      <c r="L12" s="1">
         <f t="shared" si="5"/>
         <v>280</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <f t="shared" si="6"/>
         <v>6203</v>
       </c>
-      <c r="M12" s="20"/>
       <c r="N12" s="20"/>
       <c r="O12" s="20"/>
       <c r="P12" s="20"/>
-      <c r="Q12">
+      <c r="Q12" s="20"/>
+      <c r="R12">
         <v>3</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>650</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>4</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>387</v>
       </c>
-      <c r="U12" s="20"/>
       <c r="V12" s="20"/>
-      <c r="W12" t="str">
+      <c r="W12" s="20"/>
+      <c r="X12" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X12" t="str">
-        <f t="shared" si="2"/>
-        <v>EQUAL</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26">
+      <c r="Y12" t="str">
+        <f t="shared" si="2"/>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27">
       <c r="A13" s="5">
         <v>44059</v>
       </c>
@@ -5784,68 +5830,71 @@
       <c r="C13" s="28">
         <v>44065</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13">
         <v>26</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <f t="shared" si="7"/>
         <v>14.75</v>
       </c>
-      <c r="F13" s="24">
+      <c r="G13" s="24">
         <f t="shared" si="3"/>
         <v>100.68933467585781</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>1590</v>
       </c>
-      <c r="H13" s="9">
+      <c r="I13" s="9">
         <f t="shared" si="4"/>
         <v>6157.5400821005342</v>
       </c>
-      <c r="I13" s="4">
+      <c r="J13" s="4">
         <f t="shared" si="0"/>
         <v>1.6352201257861635E-2</v>
       </c>
-      <c r="J13" s="13">
+      <c r="K13" s="13">
         <f t="shared" si="8"/>
         <v>1.3402204652808523E-2</v>
       </c>
-      <c r="K13" s="1">
+      <c r="L13" s="1">
         <f t="shared" si="5"/>
         <v>306</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <f t="shared" si="6"/>
         <v>7793</v>
       </c>
-      <c r="M13" s="20"/>
       <c r="N13" s="20"/>
       <c r="O13" s="20"/>
       <c r="P13" s="20"/>
-      <c r="Q13" s="9">
+      <c r="Q13" s="20"/>
+      <c r="R13" s="9">
         <v>4</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>470</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>22</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>1120</v>
       </c>
-      <c r="U13" s="20"/>
       <c r="V13" s="20"/>
-      <c r="W13" t="str">
+      <c r="W13" s="20"/>
+      <c r="X13" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X13" t="str">
-        <f t="shared" si="2"/>
-        <v>EQUAL</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26">
+      <c r="Y13" t="str">
+        <f t="shared" si="2"/>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27">
       <c r="A14" s="5">
         <v>44066</v>
       </c>
@@ -5855,82 +5904,85 @@
       <c r="C14" s="28">
         <v>44072</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14">
         <v>173</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <f t="shared" si="7"/>
         <v>53.25</v>
       </c>
-      <c r="F14" s="24">
+      <c r="G14" s="24">
         <f t="shared" si="3"/>
         <v>669.97134226628464</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>2188</v>
       </c>
-      <c r="H14" s="9">
+      <c r="I14" s="9">
         <f t="shared" si="4"/>
         <v>8473.3947796452649</v>
       </c>
-      <c r="I14" s="4">
+      <c r="J14" s="4">
         <f t="shared" si="0"/>
         <v>7.906764168190128E-2</v>
       </c>
-      <c r="J14" s="13">
+      <c r="K14" s="13">
         <f t="shared" si="8"/>
         <v>2.7777514619254332E-2</v>
       </c>
-      <c r="K14" s="1">
+      <c r="L14" s="1">
         <f t="shared" si="5"/>
         <v>479</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <f t="shared" si="6"/>
         <v>9981</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>67</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>271</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>106</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>1917</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>0</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>517</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>173</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>1671</v>
       </c>
-      <c r="U14" t="str">
-        <f t="shared" ref="U14:U23" si="9">IF(M14+O14=D14,"EQUAL","DIFFER")</f>
-        <v>EQUAL</v>
-      </c>
       <c r="V14" t="str">
-        <f t="shared" ref="V14:V23" si="10">IF(N14+P14=G14,"EQUAL","DIFFER")</f>
+        <f t="shared" ref="V14:V23" si="9">IF(N14+P14=E14,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="W14" t="str">
+        <f t="shared" ref="W14:W23" si="10">IF(O14+Q14=H14,"EQUAL","DIFFER")</f>
+        <v>EQUAL</v>
+      </c>
+      <c r="X14" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X14" t="str">
-        <f t="shared" si="2"/>
-        <v>EQUAL</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26">
+      <c r="Y14" t="str">
+        <f t="shared" si="2"/>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27">
       <c r="A15" s="5">
         <v>44073</v>
       </c>
@@ -5940,82 +5992,85 @@
       <c r="C15" s="28">
         <v>44079</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15">
         <v>861</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <f t="shared" si="7"/>
         <v>266.75</v>
       </c>
-      <c r="F15" s="24">
+      <c r="G15" s="24">
         <f t="shared" si="3"/>
         <v>3334.3660444582138</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>6986</v>
       </c>
-      <c r="H15" s="9">
+      <c r="I15" s="9">
         <f t="shared" si="4"/>
         <v>27054.449694059331</v>
       </c>
-      <c r="I15" s="4">
+      <c r="J15" s="4">
         <f t="shared" si="0"/>
         <v>0.12324649298597194</v>
       </c>
-      <c r="J15" s="13">
+      <c r="K15" s="13">
         <f t="shared" si="8"/>
         <v>5.6354144251443361E-2</v>
       </c>
-      <c r="K15" s="1">
+      <c r="L15" s="1">
         <f t="shared" si="5"/>
         <v>1340</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <f t="shared" si="6"/>
         <v>16967</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>310</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>662</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>551</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>6324</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>16</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>640</v>
       </c>
-      <c r="S15">
+      <c r="T15">
         <v>845</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>6346</v>
       </c>
-      <c r="U15" t="str">
+      <c r="V15" t="str">
         <f t="shared" si="9"/>
         <v>EQUAL</v>
       </c>
-      <c r="V15" t="str">
+      <c r="W15" t="str">
         <f t="shared" si="10"/>
         <v>EQUAL</v>
       </c>
-      <c r="W15" t="str">
+      <c r="X15" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X15" t="str">
-        <f t="shared" si="2"/>
-        <v>EQUAL</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26">
+      <c r="Y15" t="str">
+        <f t="shared" si="2"/>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27">
       <c r="A16" s="5">
         <v>44080</v>
       </c>
@@ -6025,82 +6080,85 @@
       <c r="C16" s="28">
         <v>44086</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16">
         <v>487</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <f t="shared" si="7"/>
         <v>386.75</v>
       </c>
-      <c r="F16" s="24">
+      <c r="G16" s="24">
         <f t="shared" si="3"/>
         <v>1885.9886918131826</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>9254</v>
       </c>
-      <c r="H16" s="9">
+      <c r="I16" s="9">
         <f t="shared" si="4"/>
         <v>35837.65781116877</v>
       </c>
-      <c r="I16" s="4">
+      <c r="J16" s="4">
         <f t="shared" si="0"/>
         <v>5.2625891506375623E-2</v>
       </c>
-      <c r="J16" s="13">
+      <c r="K16" s="13">
         <f t="shared" si="8"/>
         <v>6.7823056858027628E-2</v>
       </c>
-      <c r="K16" s="1">
+      <c r="L16" s="1">
         <f t="shared" si="5"/>
         <v>1827</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <f t="shared" si="6"/>
         <v>26221</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>111</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>334</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>376</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>8920</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>10</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>957</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>477</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>8297</v>
       </c>
-      <c r="U16" t="str">
+      <c r="V16" t="str">
         <f t="shared" si="9"/>
         <v>EQUAL</v>
       </c>
-      <c r="V16" t="str">
+      <c r="W16" t="str">
         <f t="shared" si="10"/>
         <v>EQUAL</v>
       </c>
-      <c r="W16" t="str">
+      <c r="X16" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X16" t="str">
-        <f t="shared" si="2"/>
-        <v>EQUAL</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24">
+      <c r="Y16" t="str">
+        <f t="shared" si="2"/>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25">
       <c r="A17" s="5">
         <v>44087</v>
       </c>
@@ -6110,82 +6168,85 @@
       <c r="C17" s="28">
         <v>44093</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17">
         <v>858</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <f t="shared" si="7"/>
         <v>594.75</v>
       </c>
-      <c r="F17" s="24">
+      <c r="G17" s="24">
         <f t="shared" si="3"/>
         <v>3322.7480443033073</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>19442</v>
       </c>
-      <c r="H17" s="9">
+      <c r="I17" s="9">
         <f t="shared" si="4"/>
         <v>75292.386337231816</v>
       </c>
-      <c r="I17" s="4">
+      <c r="J17" s="4">
         <f t="shared" si="0"/>
         <v>4.4131262215821421E-2</v>
       </c>
-      <c r="J17" s="13">
+      <c r="K17" s="13">
         <f t="shared" si="8"/>
         <v>7.4767822097517575E-2</v>
       </c>
-      <c r="K17" s="1">
+      <c r="L17" s="1">
         <f t="shared" si="5"/>
         <v>2685</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <f t="shared" si="6"/>
         <v>45663</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>21</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>86</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>837</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>19356</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>3</v>
       </c>
-      <c r="R17">
+      <c r="S17">
         <v>921</v>
       </c>
-      <c r="S17">
+      <c r="T17">
         <v>855</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>18521</v>
       </c>
-      <c r="U17" t="str">
+      <c r="V17" t="str">
         <f t="shared" si="9"/>
         <v>EQUAL</v>
       </c>
-      <c r="V17" t="str">
+      <c r="W17" t="str">
         <f t="shared" si="10"/>
         <v>EQUAL</v>
       </c>
-      <c r="W17" t="str">
+      <c r="X17" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X17" t="str">
-        <f t="shared" si="2"/>
-        <v>EQUAL</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24">
+      <c r="Y17" t="str">
+        <f t="shared" si="2"/>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25">
       <c r="A18" s="5">
         <v>44094</v>
       </c>
@@ -6195,82 +6256,85 @@
       <c r="C18" s="28">
         <v>44100</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18">
         <v>486</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <f t="shared" si="7"/>
         <v>673</v>
       </c>
-      <c r="F18" s="24">
+      <c r="G18" s="24">
         <f t="shared" si="3"/>
         <v>1882.1160250948803</v>
       </c>
-      <c r="G18" s="9">
+      <c r="H18" s="9">
         <v>7698</v>
       </c>
-      <c r="H18" s="9">
+      <c r="I18" s="9">
         <f t="shared" si="4"/>
         <v>29811.788397490513</v>
       </c>
-      <c r="I18" s="4">
+      <c r="J18" s="4">
         <f t="shared" si="0"/>
         <v>6.313328137178488E-2</v>
       </c>
-      <c r="J18" s="13">
+      <c r="K18" s="13">
         <f t="shared" si="8"/>
         <v>7.0784232019988472E-2</v>
       </c>
-      <c r="K18" s="1">
+      <c r="L18" s="1">
         <f t="shared" si="5"/>
         <v>3171</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <f t="shared" si="6"/>
         <v>53361</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>138</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>675</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>348</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <v>7023</v>
       </c>
-      <c r="Q18">
+      <c r="R18">
         <v>3</v>
       </c>
-      <c r="R18">
+      <c r="S18">
         <v>433</v>
       </c>
-      <c r="S18">
+      <c r="T18">
         <v>483</v>
       </c>
-      <c r="T18">
+      <c r="U18">
         <v>7265</v>
       </c>
-      <c r="U18" t="str">
+      <c r="V18" t="str">
         <f t="shared" si="9"/>
         <v>EQUAL</v>
       </c>
-      <c r="V18" t="str">
+      <c r="W18" t="str">
         <f t="shared" si="10"/>
         <v>EQUAL</v>
       </c>
-      <c r="W18" t="str">
+      <c r="X18" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X18" t="str">
-        <f t="shared" si="2"/>
-        <v>EQUAL</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24">
+      <c r="Y18" t="str">
+        <f t="shared" si="2"/>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25">
       <c r="A19" s="5">
         <v>44101</v>
       </c>
@@ -6280,82 +6344,85 @@
       <c r="C19" s="28">
         <v>44107</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19">
         <v>588</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <f t="shared" si="7"/>
         <v>604.75</v>
       </c>
-      <c r="F19" s="24">
+      <c r="G19" s="24">
         <f t="shared" si="3"/>
         <v>2277.1280303617073</v>
       </c>
-      <c r="G19" s="9">
+      <c r="H19" s="9">
         <v>8729</v>
       </c>
-      <c r="H19" s="9">
+      <c r="I19" s="9">
         <f t="shared" si="4"/>
         <v>33804.507784060108</v>
       </c>
-      <c r="I19" s="4">
+      <c r="J19" s="4">
         <f t="shared" si="0"/>
         <v>6.7361668003207698E-2</v>
       </c>
-      <c r="J19" s="13">
+      <c r="K19" s="13">
         <f t="shared" si="8"/>
         <v>5.6813025774297407E-2</v>
       </c>
-      <c r="K19" s="1">
+      <c r="L19" s="1">
         <f t="shared" si="5"/>
         <v>3759</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <f t="shared" si="6"/>
         <v>62090</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>79</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <v>177</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <v>509</v>
       </c>
-      <c r="P19">
+      <c r="Q19">
         <v>8552</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <v>10</v>
       </c>
-      <c r="R19">
+      <c r="S19">
         <v>682</v>
       </c>
-      <c r="S19">
+      <c r="T19">
         <v>578</v>
       </c>
-      <c r="T19">
+      <c r="U19">
         <v>8047</v>
       </c>
-      <c r="U19" t="str">
+      <c r="V19" t="str">
         <f t="shared" si="9"/>
         <v>EQUAL</v>
       </c>
-      <c r="V19" t="str">
+      <c r="W19" t="str">
         <f t="shared" si="10"/>
         <v>EQUAL</v>
       </c>
-      <c r="W19" t="str">
+      <c r="X19" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X19" t="str">
-        <f t="shared" ref="X19:X23" si="11">IF(T19+R19=G19,"EQUAL","DIFFER")</f>
-        <v>EQUAL</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24">
+      <c r="Y19" t="str">
+        <f t="shared" ref="Y19:Y23" si="11">IF(U19+S19=H19,"EQUAL","DIFFER")</f>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25">
       <c r="A20" s="5">
         <v>44108</v>
       </c>
@@ -6365,82 +6432,85 @@
       <c r="C20" s="28">
         <v>44114</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20">
         <v>407</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <f t="shared" si="7"/>
         <v>584.75</v>
       </c>
-      <c r="F20" s="24">
+      <c r="G20" s="24">
         <f t="shared" si="3"/>
         <v>1576.1753543490047</v>
       </c>
-      <c r="G20" s="9">
+      <c r="H20" s="9">
         <v>9224</v>
       </c>
-      <c r="H20" s="9">
+      <c r="I20" s="9">
         <f t="shared" si="4"/>
         <v>35721.477809619704</v>
       </c>
-      <c r="I20" s="4">
+      <c r="J20" s="4">
         <f t="shared" si="0"/>
         <v>4.4124024284475281E-2</v>
       </c>
-      <c r="J20" s="13">
+      <c r="K20" s="13">
         <f t="shared" si="8"/>
         <v>5.4687558968822318E-2</v>
       </c>
-      <c r="K20" s="1">
+      <c r="L20" s="1">
         <f t="shared" si="5"/>
         <v>4166</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <f t="shared" si="6"/>
         <v>71314</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>35</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>96</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <v>372</v>
       </c>
-      <c r="P20">
+      <c r="Q20">
         <v>9128</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <v>6</v>
       </c>
-      <c r="R20">
+      <c r="S20">
         <v>1168</v>
       </c>
-      <c r="S20">
+      <c r="T20">
         <v>401</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <v>8056</v>
       </c>
-      <c r="U20" t="str">
+      <c r="V20" t="str">
         <f t="shared" si="9"/>
         <v>EQUAL</v>
       </c>
-      <c r="V20" t="str">
+      <c r="W20" t="str">
         <f t="shared" si="10"/>
         <v>EQUAL</v>
       </c>
-      <c r="W20" t="str">
+      <c r="X20" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X20" t="str">
+      <c r="Y20" t="str">
         <f t="shared" si="11"/>
         <v>EQUAL</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:25">
       <c r="A21" s="26">
         <v>44115</v>
       </c>
@@ -6450,82 +6520,85 @@
       <c r="C21" s="29">
         <v>44121</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21">
         <v>249</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <f t="shared" si="7"/>
         <v>432.5</v>
       </c>
-      <c r="F21" s="24">
+      <c r="G21" s="24">
         <f t="shared" si="3"/>
         <v>964.29401285725351</v>
       </c>
-      <c r="G21" s="9">
+      <c r="H21" s="9">
         <v>9033</v>
       </c>
-      <c r="H21" s="9">
+      <c r="I21" s="9">
         <f t="shared" si="4"/>
         <v>34981.798466423978</v>
       </c>
-      <c r="I21" s="4">
+      <c r="J21" s="4">
         <f t="shared" si="0"/>
         <v>2.7565592826303553E-2</v>
       </c>
-      <c r="J21" s="13">
+      <c r="K21" s="13">
         <f t="shared" si="8"/>
         <v>5.0546141621442851E-2</v>
       </c>
-      <c r="K21" s="1">
+      <c r="L21" s="1">
         <f t="shared" si="5"/>
         <v>4415</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <f t="shared" si="6"/>
         <v>80347</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>29</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>96</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <v>220</v>
       </c>
-      <c r="P21">
+      <c r="Q21">
         <v>8937</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <v>14</v>
       </c>
-      <c r="R21">
+      <c r="S21">
         <v>1057</v>
       </c>
-      <c r="S21">
+      <c r="T21">
         <v>235</v>
       </c>
-      <c r="T21">
+      <c r="U21">
         <v>7976</v>
       </c>
-      <c r="U21" t="str">
+      <c r="V21" t="str">
         <f t="shared" si="9"/>
         <v>EQUAL</v>
       </c>
-      <c r="V21" t="str">
+      <c r="W21" t="str">
         <f t="shared" si="10"/>
         <v>EQUAL</v>
       </c>
-      <c r="W21" t="str">
+      <c r="X21" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X21" t="str">
+      <c r="Y21" t="str">
         <f t="shared" si="11"/>
         <v>EQUAL</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:25">
       <c r="A22" s="26">
         <v>44122</v>
       </c>
@@ -6535,82 +6608,85 @@
       <c r="C22" s="29">
         <v>44128</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22">
         <v>156</v>
       </c>
-      <c r="E22">
-        <f>AVERAGE(D19:D22)</f>
+      <c r="F22">
+        <f>AVERAGE(E19:E22)</f>
         <v>350</v>
       </c>
-      <c r="F22" s="24">
+      <c r="G22" s="24">
         <f t="shared" si="3"/>
         <v>604.1360080551467</v>
       </c>
-      <c r="G22" s="9">
+      <c r="H22" s="9">
         <v>10436</v>
       </c>
-      <c r="H22" s="9">
+      <c r="I22" s="9">
         <f t="shared" si="4"/>
         <v>40415.149872201997</v>
       </c>
-      <c r="I22" s="4">
+      <c r="J22" s="4">
         <f t="shared" si="0"/>
         <v>1.4948256036795707E-2</v>
       </c>
-      <c r="J22" s="13">
+      <c r="K22" s="13">
         <f t="shared" si="8"/>
         <v>3.8499885287695559E-2</v>
       </c>
-      <c r="K22" s="1">
+      <c r="L22" s="1">
         <f t="shared" si="5"/>
         <v>4571</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <f t="shared" si="6"/>
         <v>90783</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>12</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <v>57</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <v>144</v>
       </c>
-      <c r="P22">
+      <c r="Q22">
         <v>10379</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <v>22</v>
       </c>
-      <c r="R22">
+      <c r="S22">
         <v>1488</v>
       </c>
-      <c r="S22">
+      <c r="T22">
         <v>134</v>
       </c>
-      <c r="T22">
+      <c r="U22">
         <v>8948</v>
       </c>
-      <c r="U22" t="str">
+      <c r="V22" t="str">
         <f t="shared" si="9"/>
         <v>EQUAL</v>
       </c>
-      <c r="V22" t="str">
+      <c r="W22" t="str">
         <f t="shared" si="10"/>
         <v>EQUAL</v>
       </c>
-      <c r="W22" t="str">
+      <c r="X22" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X22" t="str">
+      <c r="Y22" t="str">
         <f t="shared" si="11"/>
         <v>EQUAL</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23" spans="1:25">
       <c r="A23" s="26">
         <v>44129</v>
       </c>
@@ -6620,82 +6696,85 @@
       <c r="C23" s="30">
         <v>44135</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23">
         <v>88</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <f t="shared" si="7"/>
         <v>225</v>
       </c>
-      <c r="F23" s="24">
+      <c r="G23" s="24">
         <f t="shared" si="3"/>
         <v>340.7946712105956</v>
       </c>
-      <c r="G23" s="9">
+      <c r="H23" s="9">
         <v>9624</v>
       </c>
-      <c r="H23" s="9">
+      <c r="I23" s="9">
         <f t="shared" si="4"/>
         <v>37270.544496940594</v>
       </c>
-      <c r="I23" s="4">
+      <c r="J23" s="4">
         <f t="shared" si="0"/>
         <v>9.14380714879468E-3</v>
       </c>
-      <c r="J23" s="13">
+      <c r="K23" s="13">
         <f t="shared" si="8"/>
         <v>2.3945420074092307E-2</v>
       </c>
-      <c r="K23" s="1">
+      <c r="L23" s="1">
         <f t="shared" si="5"/>
         <v>4659</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <f t="shared" si="6"/>
         <v>100407</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>4</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <v>51</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>84</v>
       </c>
-      <c r="P23">
+      <c r="Q23">
         <v>9573</v>
       </c>
-      <c r="Q23">
+      <c r="R23">
         <v>6</v>
       </c>
-      <c r="R23">
+      <c r="S23">
         <v>1434</v>
       </c>
-      <c r="S23">
+      <c r="T23">
         <v>82</v>
       </c>
-      <c r="T23">
+      <c r="U23">
         <v>8190</v>
       </c>
-      <c r="U23" t="str">
+      <c r="V23" t="str">
         <f t="shared" si="9"/>
         <v>EQUAL</v>
       </c>
-      <c r="V23" t="str">
+      <c r="W23" t="str">
         <f t="shared" si="10"/>
         <v>EQUAL</v>
       </c>
-      <c r="W23" t="str">
+      <c r="X23" t="str">
         <f t="shared" si="1"/>
         <v>EQUAL</v>
       </c>
-      <c r="X23" t="str">
+      <c r="Y23" t="str">
         <f t="shared" si="11"/>
         <v>EQUAL</v>
       </c>
     </row>
-    <row r="24" spans="1:24">
+    <row r="24" spans="1:25">
       <c r="A24" s="26">
         <v>44136</v>
       </c>
@@ -6705,107 +6784,111 @@
       <c r="C24" s="26">
         <v>44142</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24">
         <v>77</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <f t="shared" si="7"/>
         <v>142.5</v>
       </c>
-      <c r="F24" s="24">
+      <c r="G24" s="24">
         <f t="shared" si="3"/>
         <v>298.19533730927117</v>
       </c>
-      <c r="G24" s="9">
+      <c r="H24" s="9">
         <v>4938</v>
       </c>
-      <c r="H24" s="9">
+      <c r="I24" s="9">
         <f t="shared" si="4"/>
         <v>19123.228254976377</v>
       </c>
-      <c r="I24" s="4">
+      <c r="J24" s="4">
         <f t="shared" si="0"/>
         <v>1.5593357634669907E-2</v>
       </c>
-      <c r="J24" s="13">
+      <c r="K24" s="13">
         <f t="shared" si="8"/>
         <v>1.6812753411640961E-2</v>
       </c>
-      <c r="K24" s="1">
+      <c r="L24" s="1">
         <f t="shared" si="5"/>
         <v>4736</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <f t="shared" si="6"/>
         <v>105345</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>2</v>
       </c>
-      <c r="N24">
+      <c r="O24">
         <v>24</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <v>75</v>
       </c>
-      <c r="P24">
+      <c r="Q24">
         <v>4914</v>
       </c>
-      <c r="Q24">
+      <c r="R24">
         <v>6</v>
       </c>
-      <c r="R24">
+      <c r="S24">
         <v>881</v>
       </c>
-      <c r="S24">
+      <c r="T24">
         <v>71</v>
       </c>
-      <c r="T24">
+      <c r="U24">
         <v>4057</v>
       </c>
-      <c r="U24" t="str">
-        <f t="shared" ref="U24" si="12">IF(M24+O24=D24,"EQUAL","DIFFER")</f>
-        <v>EQUAL</v>
-      </c>
       <c r="V24" t="str">
-        <f t="shared" ref="V24" si="13">IF(N24+P24=G24,"EQUAL","DIFFER")</f>
+        <f t="shared" ref="V24" si="12">IF(N24+P24=E24,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="W24" t="str">
-        <f t="shared" ref="W24" si="14">IF(S24+Q24=D24,"EQUAL","DIFFER")</f>
+        <f t="shared" ref="W24" si="13">IF(O24+Q24=H24,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="X24" t="str">
-        <f t="shared" ref="X24" si="15">IF(T24+R24=G24,"EQUAL","DIFFER")</f>
-        <v>EQUAL</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24">
+        <f t="shared" ref="X24" si="14">IF(T24+R24=E24,"EQUAL","DIFFER")</f>
+        <v>EQUAL</v>
+      </c>
+      <c r="Y24" t="str">
+        <f t="shared" ref="Y24" si="15">IF(U24+S24=H24,"EQUAL","DIFFER")</f>
+        <v>EQUAL</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="U1:X1 U17:X1048576">
+  <conditionalFormatting sqref="V1:Y1 V17:Y1048576">
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="DIFFER">
-      <formula>NOT(ISERROR(SEARCH("DIFFER",U1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DIFFER",V1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="EQUAL">
-      <formula>NOT(ISERROR(SEARCH("EQUAL",U1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EQUAL",V1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:X16">
+  <conditionalFormatting sqref="V2:Y16">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="DIFFER">
-      <formula>NOT(ISERROR(SEARCH("DIFFER",U2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DIFFER",V2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="EQUAL">
-      <formula>NOT(ISERROR(SEARCH("EQUAL",U2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EQUAL",V2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="E5:E24" formulaRange="1"/>
+    <ignoredError sqref="F5:F24" formulaRange="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update data and verify historical data for accuracy
</commit_message>
<xml_diff>
--- a/clemsonDashboard.xlsx
+++ b/clemsonDashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidferrara/Documents/Clemson/The Tiger/COVID-19/Data/ttn-clemson-covid-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC8B72A-88BA-7747-835B-3C3A40D74A1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2733A974-E284-8C4C-9824-3BAB6E993F2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="460" windowWidth="28040" windowHeight="16260" xr2:uid="{663FE1B6-0B7E-E04A-924C-6AB15F4F5852}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="18000" activeTab="1" xr2:uid="{663FE1B6-0B7E-E04A-924C-6AB15F4F5852}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Data" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -275,6 +275,9 @@
   <si>
     <t>End Reporting by The Tiger News</t>
   </si>
+  <si>
+    <t>CSP Since IPI</t>
+  </si>
 </sst>
 </file>
 
@@ -393,7 +396,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -445,6 +448,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -823,7 +830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2018E299-360B-F244-BDDD-9B449D0B7C0F}">
   <dimension ref="A1:X72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
@@ -4921,10 +4928,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D56922A-034D-7E4D-80AB-A29316427207}">
-  <dimension ref="A1:AC25"/>
+  <dimension ref="A1:AD25"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="95" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4953,11 +4960,12 @@
     <col min="24" max="24" width="16.6640625" customWidth="1"/>
     <col min="25" max="25" width="13.1640625" customWidth="1"/>
     <col min="26" max="26" width="24.33203125" customWidth="1"/>
-    <col min="27" max="27" width="17.33203125" customWidth="1"/>
-    <col min="28" max="28" width="18.1640625" customWidth="1"/>
+    <col min="27" max="27" width="11.5" customWidth="1"/>
+    <col min="28" max="28" width="17.33203125" customWidth="1"/>
+    <col min="29" max="29" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="17" customHeight="1">
+    <row r="1" spans="1:30" ht="17" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -5037,13 +5045,16 @@
         <v>41</v>
       </c>
       <c r="AA1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="17" customHeight="1">
+    <row r="2" spans="1:30" ht="17" customHeight="1">
       <c r="A2" s="25">
         <v>43987</v>
       </c>
@@ -5072,7 +5083,7 @@
         <v>158.77933545039113</v>
       </c>
       <c r="J2" s="4">
-        <f t="shared" ref="J2:J24" si="0">E2/H2</f>
+        <f t="shared" ref="J2:J25" si="0">E2/H2</f>
         <v>2.4390243902439025E-2</v>
       </c>
       <c r="K2" s="23"/>
@@ -5114,18 +5125,19 @@
         <f>T2</f>
         <v>1</v>
       </c>
-      <c r="AA2">
+      <c r="AA2" s="34"/>
+      <c r="AB2">
         <v>25822</v>
       </c>
-      <c r="AB2" s="32">
-        <f>Z2/AA2</f>
+      <c r="AC2" s="32">
+        <f>Z2/AB2</f>
         <v>3.872666718302223E-5</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:30">
       <c r="A3" s="5">
         <v>43989</v>
       </c>
@@ -5143,14 +5155,14 @@
       </c>
       <c r="F3" s="20"/>
       <c r="G3" s="24">
-        <f t="shared" ref="G3:G24" si="3">(E3/25822)*100000</f>
+        <f t="shared" ref="G3:G25" si="3">(E3/25822)*100000</f>
         <v>15.490666873208893</v>
       </c>
       <c r="H3">
         <v>143</v>
       </c>
       <c r="I3" s="9">
-        <f t="shared" ref="I3:I24" si="4">(H3/25822)*100000</f>
+        <f t="shared" ref="I3:I25" si="4">(H3/25822)*100000</f>
         <v>553.79134071721785</v>
       </c>
       <c r="J3" s="4">
@@ -5159,7 +5171,7 @@
       </c>
       <c r="K3" s="23"/>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L24" si="5">E3+L2</f>
+        <f t="shared" ref="L3:L25" si="5">E3+L2</f>
         <v>5</v>
       </c>
       <c r="M3">
@@ -5196,18 +5208,19 @@
         <f>Z2+T3</f>
         <v>5</v>
       </c>
-      <c r="AA3">
+      <c r="AA3" s="34"/>
+      <c r="AB3">
         <v>25822</v>
       </c>
-      <c r="AB3" s="32">
-        <f t="shared" ref="AB3:AB24" si="6">Z3/AA3</f>
+      <c r="AC3" s="32">
+        <f t="shared" ref="AC3:AC24" si="6">Z3/AB3</f>
         <v>1.9363333591511115E-4</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:30">
       <c r="A4" s="5">
         <v>43996</v>
       </c>
@@ -5245,7 +5258,7 @@
         <v>92</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M24" si="7">H4+M3</f>
+        <f t="shared" ref="M4:M25" si="7">H4+M3</f>
         <v>461</v>
       </c>
       <c r="N4" s="20"/>
@@ -5278,15 +5291,16 @@
         <f t="shared" ref="Z4:Z24" si="8">Z3+T4</f>
         <v>90</v>
       </c>
-      <c r="AA4">
+      <c r="AA4" s="34"/>
+      <c r="AB4">
         <v>25822</v>
       </c>
-      <c r="AB4" s="32">
+      <c r="AC4" s="32">
         <f t="shared" si="6"/>
         <v>3.4854000464720008E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:30">
       <c r="A5" s="5">
         <v>44003</v>
       </c>
@@ -5363,18 +5377,19 @@
         <f t="shared" si="8"/>
         <v>135</v>
       </c>
-      <c r="AA5">
+      <c r="AA5" s="34"/>
+      <c r="AB5">
         <v>25822</v>
       </c>
-      <c r="AB5" s="32">
+      <c r="AC5" s="32">
         <f t="shared" si="6"/>
         <v>5.2281000697080009E-3</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:30">
       <c r="A6" s="5">
         <v>44010</v>
       </c>
@@ -5391,7 +5406,7 @@
         <v>29</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F24" si="9">AVERAGE(E3:E6)</f>
+        <f t="shared" ref="F6:F25" si="9">AVERAGE(E3:E6)</f>
         <v>41.5</v>
       </c>
       <c r="G6" s="24">
@@ -5410,7 +5425,7 @@
         <v>0.19463087248322147</v>
       </c>
       <c r="K6" s="13">
-        <f t="shared" ref="K6:K24" si="10">AVERAGE(J3:J6)</f>
+        <f t="shared" ref="K6:K25" si="10">AVERAGE(J3:J6)</f>
         <v>0.17276118473632587</v>
       </c>
       <c r="L6" s="1">
@@ -5451,18 +5466,19 @@
         <f t="shared" si="8"/>
         <v>160</v>
       </c>
-      <c r="AA6">
+      <c r="AA6" s="34"/>
+      <c r="AB6">
         <v>25822</v>
       </c>
-      <c r="AB6" s="32">
+      <c r="AC6" s="32">
         <f t="shared" si="6"/>
         <v>6.1962667492835568E-3</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:30">
       <c r="A7" s="5">
         <v>44017</v>
       </c>
@@ -5539,15 +5555,16 @@
         <f t="shared" si="8"/>
         <v>172</v>
       </c>
-      <c r="AA7">
+      <c r="AA7" s="34"/>
+      <c r="AB7">
         <v>25822</v>
       </c>
-      <c r="AB7" s="32">
+      <c r="AC7" s="32">
         <f t="shared" si="6"/>
         <v>6.6609867554798235E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:30">
       <c r="A8" s="5">
         <v>44024</v>
       </c>
@@ -5624,15 +5641,16 @@
         <f t="shared" si="8"/>
         <v>181</v>
       </c>
-      <c r="AA8">
+      <c r="AA8" s="34"/>
+      <c r="AB8">
         <v>25822</v>
       </c>
-      <c r="AB8" s="32">
+      <c r="AC8" s="32">
         <f t="shared" si="6"/>
         <v>7.0095267601270233E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:30">
       <c r="A9" s="5">
         <v>44031</v>
       </c>
@@ -5709,15 +5727,16 @@
         <f t="shared" si="8"/>
         <v>201</v>
       </c>
-      <c r="AA9">
+      <c r="AA9" s="34"/>
+      <c r="AB9">
         <v>25822</v>
       </c>
-      <c r="AB9" s="32">
+      <c r="AC9" s="32">
         <f t="shared" si="6"/>
         <v>7.784060103787468E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:30">
       <c r="A10" s="5">
         <v>44038</v>
       </c>
@@ -5794,15 +5813,16 @@
         <f t="shared" si="8"/>
         <v>211</v>
       </c>
-      <c r="AA10">
+      <c r="AA10" s="34"/>
+      <c r="AB10">
         <v>25822</v>
       </c>
-      <c r="AB10" s="32">
+      <c r="AC10" s="32">
         <f t="shared" si="6"/>
         <v>8.1713267756176912E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:30">
       <c r="A11" s="5">
         <v>44045</v>
       </c>
@@ -5879,15 +5899,16 @@
         <f t="shared" si="8"/>
         <v>216</v>
       </c>
-      <c r="AA11">
+      <c r="AA11" s="34"/>
+      <c r="AB11">
         <v>25822</v>
       </c>
-      <c r="AB11" s="32">
+      <c r="AC11" s="32">
         <f t="shared" si="6"/>
         <v>8.3649601115328015E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:30">
       <c r="A12" s="5">
         <v>44052</v>
       </c>
@@ -5964,15 +5985,16 @@
         <f t="shared" si="8"/>
         <v>220</v>
       </c>
-      <c r="AA12">
+      <c r="AA12" s="34"/>
+      <c r="AB12">
         <v>25822</v>
       </c>
-      <c r="AB12" s="32">
+      <c r="AC12" s="32">
         <f t="shared" si="6"/>
         <v>8.5198667802648901E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:30">
       <c r="A13" s="5">
         <v>44059</v>
       </c>
@@ -6049,15 +6071,16 @@
         <f t="shared" si="8"/>
         <v>242</v>
       </c>
-      <c r="AA13">
+      <c r="AA13" s="34"/>
+      <c r="AB13">
         <v>25822</v>
       </c>
-      <c r="AB13" s="32">
+      <c r="AC13" s="32">
         <f t="shared" si="6"/>
         <v>9.37185345829138E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:30">
       <c r="A14" s="5">
         <v>44066</v>
       </c>
@@ -6148,15 +6171,16 @@
         <f t="shared" si="8"/>
         <v>415</v>
       </c>
-      <c r="AA14">
+      <c r="AA14" s="34"/>
+      <c r="AB14">
         <v>25822</v>
       </c>
-      <c r="AB14" s="32">
+      <c r="AC14" s="32">
         <f t="shared" si="6"/>
         <v>1.6071566880954225E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:30">
       <c r="A15" s="5">
         <v>44073</v>
       </c>
@@ -6247,15 +6271,16 @@
         <f t="shared" si="8"/>
         <v>1260</v>
       </c>
-      <c r="AA15">
+      <c r="AA15" s="34"/>
+      <c r="AB15">
         <v>25822</v>
       </c>
-      <c r="AB15" s="32">
+      <c r="AC15" s="32">
         <f t="shared" si="6"/>
         <v>4.8795600650608006E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:30">
       <c r="A16" s="5">
         <v>44080</v>
       </c>
@@ -6346,15 +6371,16 @@
         <f t="shared" si="8"/>
         <v>1737</v>
       </c>
-      <c r="AA16">
+      <c r="AA16" s="34"/>
+      <c r="AB16">
         <v>25822</v>
       </c>
-      <c r="AB16" s="32">
+      <c r="AC16" s="32">
         <f t="shared" si="6"/>
         <v>6.7268220896909606E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:29">
       <c r="A17" s="5">
         <v>44087</v>
       </c>
@@ -6445,15 +6471,16 @@
         <f t="shared" si="8"/>
         <v>2592</v>
       </c>
-      <c r="AA17">
+      <c r="AA17" s="34"/>
+      <c r="AB17">
         <v>25822</v>
       </c>
-      <c r="AB17" s="32">
+      <c r="AC17" s="32">
         <f t="shared" si="6"/>
         <v>0.10037952133839362</v>
       </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:29">
       <c r="A18" s="5">
         <v>44094</v>
       </c>
@@ -6545,14 +6572,18 @@
         <v>3075</v>
       </c>
       <c r="AA18">
+        <f>T18</f>
+        <v>483</v>
+      </c>
+      <c r="AB18">
         <v>25822</v>
       </c>
-      <c r="AB18" s="32">
+      <c r="AC18" s="32">
         <f t="shared" si="6"/>
         <v>0.11908450158779335</v>
       </c>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:29">
       <c r="A19" s="5">
         <v>44101</v>
       </c>
@@ -6644,14 +6675,18 @@
         <v>3653</v>
       </c>
       <c r="AA19">
+        <f>AA18+T19</f>
+        <v>1061</v>
+      </c>
+      <c r="AB19">
         <v>25822</v>
       </c>
-      <c r="AB19" s="32">
+      <c r="AC19" s="32">
         <f t="shared" si="6"/>
         <v>0.1414685152195802</v>
       </c>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:29">
       <c r="A20" s="5">
         <v>44108</v>
       </c>
@@ -6743,21 +6778,25 @@
         <v>4054</v>
       </c>
       <c r="AA20">
+        <f t="shared" ref="AA20:AA25" si="14">AA19+T20</f>
+        <v>1462</v>
+      </c>
+      <c r="AB20">
         <v>25822</v>
       </c>
-      <c r="AB20" s="32">
+      <c r="AC20" s="32">
         <f t="shared" si="6"/>
         <v>0.1569979087599721</v>
       </c>
     </row>
-    <row r="21" spans="1:28">
-      <c r="A21" s="26">
+    <row r="21" spans="1:29">
+      <c r="A21" s="5">
         <v>44115</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="29">
+      <c r="C21" s="28">
         <v>44121</v>
       </c>
       <c r="D21" s="31" t="s">
@@ -6842,14 +6881,18 @@
         <v>4289</v>
       </c>
       <c r="AA21">
+        <f t="shared" si="14"/>
+        <v>1697</v>
+      </c>
+      <c r="AB21">
         <v>25822</v>
       </c>
-      <c r="AB21" s="32">
+      <c r="AC21" s="32">
         <f t="shared" si="6"/>
         <v>0.16609867554798233</v>
       </c>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:29">
       <c r="A22" s="26">
         <v>44122</v>
       </c>
@@ -6863,38 +6906,38 @@
         <v>38</v>
       </c>
       <c r="E22">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F22">
         <f>AVERAGE(E19:E22)</f>
-        <v>350</v>
+        <v>350.5</v>
       </c>
       <c r="G22" s="24">
         <f t="shared" si="3"/>
-        <v>604.1360080551467</v>
+        <v>611.8813414917513</v>
       </c>
       <c r="H22" s="9">
-        <v>10436</v>
+        <v>10686</v>
       </c>
       <c r="I22" s="9">
         <f t="shared" si="4"/>
-        <v>40415.149872201997</v>
+        <v>41383.316551777556</v>
       </c>
       <c r="J22" s="4">
         <f t="shared" si="0"/>
-        <v>1.4948256036795707E-2</v>
+        <v>1.4785700917087778E-2</v>
       </c>
       <c r="K22" s="13">
         <f t="shared" si="10"/>
-        <v>3.8497597306883284E-2</v>
+        <v>3.8456958526956304E-2</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" si="5"/>
-        <v>4571</v>
+        <v>4573</v>
       </c>
       <c r="M22">
         <f t="shared" si="7"/>
-        <v>90786</v>
+        <v>91036</v>
       </c>
       <c r="N22">
         <v>12</v>
@@ -6903,22 +6946,22 @@
         <v>57</v>
       </c>
       <c r="P22">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="Q22">
-        <v>10379</v>
+        <v>10629</v>
       </c>
       <c r="R22">
         <v>22</v>
       </c>
       <c r="S22">
-        <v>1488</v>
+        <v>1726</v>
       </c>
       <c r="T22">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="U22">
-        <v>8948</v>
+        <v>8960</v>
       </c>
       <c r="V22" t="str">
         <f t="shared" si="11"/>
@@ -6938,17 +6981,21 @@
       </c>
       <c r="Z22">
         <f t="shared" si="8"/>
-        <v>4423</v>
+        <v>4425</v>
       </c>
       <c r="AA22">
+        <f t="shared" si="14"/>
+        <v>1833</v>
+      </c>
+      <c r="AB22">
         <v>25822</v>
       </c>
-      <c r="AB22" s="32">
+      <c r="AC22" s="32">
         <f t="shared" si="6"/>
-        <v>0.17128804895050731</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28">
+        <v>0.17136550228487335</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29">
       <c r="A23" s="26">
         <v>44129</v>
       </c>
@@ -6962,38 +7009,38 @@
         <v>38</v>
       </c>
       <c r="E23">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="F23">
         <f t="shared" si="9"/>
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="G23" s="24">
         <f t="shared" si="3"/>
-        <v>340.7946712105956</v>
+        <v>364.03067152040893</v>
       </c>
       <c r="H23" s="9">
-        <v>9624</v>
+        <v>9675</v>
       </c>
       <c r="I23" s="9">
         <f t="shared" si="4"/>
-        <v>37270.544496940594</v>
+        <v>37468.050499574005</v>
       </c>
       <c r="J23" s="4">
         <f t="shared" si="0"/>
-        <v>9.14380714879468E-3</v>
+        <v>9.7157622739018085E-3</v>
       </c>
       <c r="K23" s="13">
         <f t="shared" si="10"/>
-        <v>2.3943132093280028E-2</v>
+        <v>2.4045482094629828E-2</v>
       </c>
       <c r="L23" s="1">
         <f t="shared" si="5"/>
-        <v>4659</v>
+        <v>4667</v>
       </c>
       <c r="M23">
         <f t="shared" si="7"/>
-        <v>100410</v>
+        <v>100711</v>
       </c>
       <c r="N23">
         <v>4</v>
@@ -7002,22 +7049,22 @@
         <v>51</v>
       </c>
       <c r="P23">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="Q23">
-        <v>9573</v>
+        <v>9624</v>
       </c>
       <c r="R23">
         <v>6</v>
       </c>
       <c r="S23">
-        <v>1434</v>
+        <v>1440</v>
       </c>
       <c r="T23">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="U23">
-        <v>8190</v>
+        <v>8235</v>
       </c>
       <c r="V23" t="str">
         <f t="shared" si="11"/>
@@ -7037,21 +7084,25 @@
       </c>
       <c r="Z23">
         <f t="shared" si="8"/>
-        <v>4505</v>
+        <v>4513</v>
       </c>
       <c r="AA23">
+        <f t="shared" si="14"/>
+        <v>1921</v>
+      </c>
+      <c r="AB23">
         <v>25822</v>
       </c>
-      <c r="AB23" s="32">
+      <c r="AC23" s="32">
         <f t="shared" si="6"/>
-        <v>0.17446363565951514</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28">
+        <v>0.17477344899697933</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29">
       <c r="A24" s="26">
         <v>44136</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="33" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="26">
@@ -7061,100 +7112,201 @@
         <v>38</v>
       </c>
       <c r="E24">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="F24">
         <f t="shared" si="9"/>
-        <v>142.5</v>
+        <v>151.5</v>
       </c>
       <c r="G24" s="24">
         <f t="shared" si="3"/>
-        <v>298.19533730927117</v>
+        <v>406.63000542173342</v>
       </c>
       <c r="H24" s="9">
-        <v>4938</v>
+        <v>7757</v>
       </c>
       <c r="I24" s="9">
         <f t="shared" si="4"/>
-        <v>19123.228254976377</v>
+        <v>30040.275733870341</v>
       </c>
       <c r="J24" s="4">
         <f t="shared" si="0"/>
-        <v>1.5593357634669907E-2</v>
+        <v>1.3536160886940828E-2</v>
       </c>
       <c r="K24" s="13">
         <f t="shared" si="10"/>
-        <v>1.6810465430828685E-2</v>
+        <v>1.6398516245246214E-2</v>
       </c>
       <c r="L24" s="1">
         <f t="shared" si="5"/>
-        <v>4736</v>
+        <v>4772</v>
       </c>
       <c r="M24">
         <f t="shared" si="7"/>
-        <v>105348</v>
+        <v>108468</v>
       </c>
       <c r="N24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O24">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="P24">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="Q24">
-        <v>4914</v>
+        <v>7712</v>
       </c>
       <c r="R24">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S24">
-        <v>881</v>
+        <v>915</v>
       </c>
       <c r="T24">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="U24">
-        <v>4057</v>
+        <v>6842</v>
       </c>
       <c r="V24" t="str">
-        <f t="shared" ref="V24" si="14">IF(N24+P24=E24,"EQUAL","DIFFER")</f>
+        <f t="shared" ref="V24" si="15">IF(N24+P24=E24,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="W24" t="str">
-        <f t="shared" ref="W24" si="15">IF(O24+Q24=H24,"EQUAL","DIFFER")</f>
+        <f t="shared" ref="W24" si="16">IF(O24+Q24=H24,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="X24" t="str">
-        <f t="shared" ref="X24" si="16">IF(T24+R24=E24,"EQUAL","DIFFER")</f>
+        <f t="shared" ref="X24" si="17">IF(T24+R24=E24,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="Y24" t="str">
-        <f t="shared" ref="Y24" si="17">IF(U24+S24=H24,"EQUAL","DIFFER")</f>
+        <f t="shared" ref="Y24" si="18">IF(U24+S24=H24,"EQUAL","DIFFER")</f>
         <v>EQUAL</v>
       </c>
       <c r="Z24">
         <f t="shared" si="8"/>
-        <v>4576</v>
+        <v>4613</v>
       </c>
       <c r="AA24">
+        <f t="shared" si="14"/>
+        <v>2021</v>
+      </c>
+      <c r="AB24">
         <v>25822</v>
       </c>
-      <c r="AB24" s="32">
+      <c r="AC24" s="32">
         <f t="shared" si="6"/>
-        <v>0.17721322902950973</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+        <v>0.17864611571528155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29">
+      <c r="A25" s="26">
+        <v>44143</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="26">
+        <v>44139</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25">
+        <v>88</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="9"/>
+        <v>111.25</v>
+      </c>
+      <c r="G25" s="24">
+        <f t="shared" si="3"/>
+        <v>340.7946712105956</v>
+      </c>
+      <c r="H25" s="9">
+        <v>8844</v>
+      </c>
+      <c r="I25" s="9">
+        <f t="shared" si="4"/>
+        <v>34249.864456664858</v>
+      </c>
+      <c r="J25" s="4">
+        <f t="shared" si="0"/>
+        <v>9.9502487562189053E-3</v>
+      </c>
+      <c r="K25" s="13">
+        <f t="shared" si="10"/>
+        <v>1.199696820853733E-2</v>
+      </c>
+      <c r="L25" s="1">
+        <f t="shared" si="5"/>
+        <v>4860</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="7"/>
+        <v>117312</v>
+      </c>
+      <c r="N25">
+        <v>3</v>
+      </c>
+      <c r="O25">
+        <v>19</v>
+      </c>
+      <c r="P25">
+        <v>85</v>
+      </c>
+      <c r="Q25">
+        <v>8825</v>
+      </c>
+      <c r="R25">
+        <v>7</v>
+      </c>
+      <c r="S25">
+        <v>1498</v>
+      </c>
+      <c r="T25">
+        <v>81</v>
+      </c>
+      <c r="U25">
+        <v>7346</v>
+      </c>
+      <c r="V25" t="str">
+        <f t="shared" ref="V25" si="19">IF(N25+P25=E25,"EQUAL","DIFFER")</f>
+        <v>EQUAL</v>
+      </c>
+      <c r="W25" t="str">
+        <f t="shared" ref="W25" si="20">IF(O25+Q25=H25,"EQUAL","DIFFER")</f>
+        <v>EQUAL</v>
+      </c>
+      <c r="X25" t="str">
+        <f t="shared" ref="X25" si="21">IF(T25+R25=E25,"EQUAL","DIFFER")</f>
+        <v>EQUAL</v>
+      </c>
+      <c r="Y25" t="str">
+        <f t="shared" ref="Y25" si="22">IF(U25+S25=H25,"EQUAL","DIFFER")</f>
+        <v>EQUAL</v>
+      </c>
+      <c r="Z25">
+        <f t="shared" ref="Z25" si="23">Z24+T25</f>
+        <v>4694</v>
+      </c>
+      <c r="AA25">
+        <f t="shared" si="14"/>
+        <v>2102</v>
+      </c>
+      <c r="AB25">
+        <v>25822</v>
+      </c>
+      <c r="AC25" s="32">
+        <f t="shared" ref="AC25" si="24">Z25/AB25</f>
+        <v>0.18178297575710634</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="V25:AA1048576 V17:Y24 V1:AB1">
+  <conditionalFormatting sqref="V26:AB1048576 V1:AC1 V17:Y25">
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="DIFFER">
       <formula>NOT(ISERROR(SEARCH("DIFFER",V1)))</formula>
     </cfRule>
@@ -7162,7 +7314,7 @@
       <formula>NOT(ISERROR(SEARCH("EQUAL",V1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V2:AA2 V3:Z3 AA3:AA24 V4:Y16 Z4:Z24">
+  <conditionalFormatting sqref="V2:AB2 V3:AA3 V4:Y16 AB3:AB25 Z4:AA25">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="DIFFER">
       <formula>NOT(ISERROR(SEARCH("DIFFER",V2)))</formula>
     </cfRule>
@@ -7180,7 +7332,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE67BA8-2D94-544F-9655-C971E88AFA0C}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView zoomScale="138" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
@@ -7248,7 +7400,7 @@
         <v>289</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D14" si="0">B5+C5</f>
+        <f t="shared" ref="D5:D15" si="0">B5+C5</f>
         <v>532</v>
       </c>
     </row>
@@ -7385,6 +7537,21 @@
       <c r="D14">
         <f t="shared" si="0"/>
         <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2">
+        <v>44147</v>
+      </c>
+      <c r="B15" s="9">
+        <v>43</v>
+      </c>
+      <c r="C15">
+        <v>54</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>